<commit_message>
done CESE and PADI species
</commit_message>
<xml_diff>
--- a/data/Kleaf_Karli_Marion_CESE.xlsx
+++ b/data/Kleaf_Karli_Marion_CESE.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marion.boisseaux\Dropbox\Mon PC (Jaboty20)\Post_doc_CalState_LA\ScoffoniLab_Kleaf\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E16AAEE-FDE6-4AFE-ADCE-EAB5326A7098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0468CD7-2961-4D84-91EE-825748F344BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{63D1BA6E-C94C-4260-825C-85D06C6809A1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{63D1BA6E-C94C-4260-825C-85D06C6809A1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="CESE" sheetId="1" r:id="rId1"/>
+    <sheet name="PADI" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AE$23</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CESE!$A$1:$AE$23</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="39">
   <si>
     <t>Specie</t>
   </si>
@@ -148,6 +149,15 @@
   <si>
     <t>ok</t>
   </si>
+  <si>
+    <t>middle water potential 1.757 but side water potential 0.613</t>
+  </si>
+  <si>
+    <t>PADI</t>
+  </si>
+  <si>
+    <t>could not do the potential, the leaf broke while doing it</t>
+  </si>
 </sst>
 </file>
 
@@ -185,7 +195,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -204,6 +214,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -217,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -234,6 +250,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -326,12 +347,62 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.3332422979095855E-2"/>
+                  <c:y val="-0.48586097519703042"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-150"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$X$3:$X$28</c:f>
+              <c:f>CESE!$X$3:$X$30</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>0.155</c:v>
                 </c:pt>
@@ -363,62 +434,68 @@
                   <c:v>0.39700000000000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>0.25600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.40699999999999997</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>0.23</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>0.73</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
                   <c:v>0.22</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
                   <c:v>0.28000000000000003</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="17">
                   <c:v>1.96</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="18">
                   <c:v>0.06</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="19">
                   <c:v>0.39400000000000002</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="20">
                   <c:v>0.05</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="21">
                   <c:v>0.25800000000000001</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="22">
                   <c:v>0.63500000000000001</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="23">
                   <c:v>0.89</c:v>
                 </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.25600000000000001</c:v>
-                </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="24">
                   <c:v>1.4770000000000001</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="25">
                   <c:v>0.39300000000000002</c:v>
                 </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.40699999999999997</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.2</c:v>
+                <c:pt idx="26">
+                  <c:v>1.7569999999999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.83299999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$W$3:$W$28</c:f>
+              <c:f>CESE!$W$3:$W$30</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>7.3619320095278127</c:v>
                 </c:pt>
@@ -450,52 +527,55 @@
                   <c:v>2.1531427937055092</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>13.884159288295567</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.1994102626647241</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11.498389608227583</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>10.037452030841736</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>3.3065983252733466</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
                   <c:v>8.3428226636098692</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
                   <c:v>12.796323814364923</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="17">
                   <c:v>0.77904348189660955</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="18">
                   <c:v>33.786613558198361</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="19">
                   <c:v>6.4782847510677168</c:v>
                 </c:pt>
-                <c:pt idx="17">
-                  <c:v>60.139863517462565</c:v>
-                </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="21">
                   <c:v>5.0367789985377067</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="22">
                   <c:v>0.13757458189717575</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="23">
                   <c:v>1.694071098222929</c:v>
                 </c:pt>
-                <c:pt idx="21">
-                  <c:v>13.884159288295567</c:v>
-                </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="24">
                   <c:v>2.3612189931130394</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="25">
                   <c:v>3.9071513834929439</c:v>
                 </c:pt>
-                <c:pt idx="24">
-                  <c:v>4.1994102626647241</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>11.498389608227583</c:v>
+                <c:pt idx="26">
+                  <c:v>2.2213417198360363</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.7391231388436081</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -809,10 +889,430 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-150"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Kleaf</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>PADI!$X$3:$X$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.92400000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.9000000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.075</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.8000000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.95899999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.27800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.92500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.21099999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.88400000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.68799999999999994</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.7000000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.11700000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>PADI!$W$3:$W$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1.6588820843428438</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>75.374833526691248</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.6019228638124352</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30.46140123557058</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.458878537998741</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.88420649912393312</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.552298839107099</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.6430951275139472</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.75951343974434249</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14.810455045659179</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.2503816096316034</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.942767763669117</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40.509885266170855</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>29.455391836261956</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.9253041603633623</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-F1D5-4973-A265-7DEF7E3FF39F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1645049087"/>
+        <c:axId val="1645017407"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1645049087"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-150"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1645017407"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1645017407"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-150"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1645049087"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-150"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
   <a:schemeClr val="accent2"/>
   <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
@@ -1362,20 +1862,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>274320</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>586740</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>49530</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>398145</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>81915</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1383,6 +2399,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99B17855-78F2-2E0D-D667-BEB0AC0485D0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>49530</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>49530</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Graphique 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B65154C-BAED-2069-6405-9AC9357BBEBD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1700,11 +2757,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3FF746F-B21E-4AE2-A531-A971B17E5B05}">
-  <dimension ref="A1:AE28"/>
+  <dimension ref="A1:AE30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z30" sqref="Z30"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1720,6 +2777,7 @@
     <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.21875" customWidth="1"/>
     <col min="14" max="14" width="5.5546875" customWidth="1"/>
+    <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.3">
@@ -1878,15 +2936,15 @@
         <v>7.9901147959183669</v>
       </c>
       <c r="V2" s="4">
-        <f t="shared" ref="V2:V23" si="0">I2*0.000001/18*1000/R2/(U2/10000)</f>
+        <f t="shared" ref="V2:V28" si="0">I2*0.000001/18*1000/R2/(U2/10000)</f>
         <v>3.2285263672899864</v>
       </c>
       <c r="W2" s="4">
-        <f t="shared" ref="W2:W23" si="1">V2/(0.88862*(1/POWER(10,(1.3272*(20-K2)-0.001053*(K2-20)^2)/(K2+105))))</f>
+        <f t="shared" ref="W2:W22" si="1">V2/(0.88862*(1/POWER(10,(1.3272*(20-K2)-0.001053*(K2-20)^2)/(K2+105))))</f>
         <v>3.589207007751122</v>
       </c>
       <c r="X2" s="4">
-        <f t="shared" ref="X2:X23" si="2">MAX(Q2:R2)</f>
+        <f t="shared" ref="X2:X30" si="2">MAX(Q2:R2)</f>
         <v>0.48499999999999999</v>
       </c>
       <c r="Z2" t="s">
@@ -1954,7 +3012,7 @@
         <v>2745160</v>
       </c>
       <c r="U3" s="4">
-        <f t="shared" ref="U3:U23" si="3">S3/(1200^2)*2.54^2</f>
+        <f t="shared" ref="U3:U28" si="3">S3/(1200^2)*2.54^2</f>
         <v>12.299079344444445</v>
       </c>
       <c r="V3" s="4">
@@ -2531,189 +3589,170 @@
         <v>27</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E13">
-        <v>10222024</v>
+        <v>1112024</v>
       </c>
       <c r="F13" s="5">
-        <v>0.48958333333333331</v>
+        <v>0.4777777777777778</v>
       </c>
       <c r="G13" s="5">
-        <v>0.46458333333333335</v>
+        <v>0.49444444444444446</v>
       </c>
       <c r="H13" t="s">
         <v>28</v>
       </c>
       <c r="I13">
-        <v>35.78</v>
+        <v>23</v>
       </c>
       <c r="J13">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="K13" s="2">
-        <v>25.5</v>
-      </c>
-      <c r="M13" s="2"/>
-      <c r="Q13" s="4"/>
+        <v>0.05</v>
+      </c>
+      <c r="K13">
+        <v>25</v>
+      </c>
       <c r="R13">
-        <v>0.23</v>
+        <v>0.25600000000000001</v>
       </c>
       <c r="S13">
-        <f>758232+749922+344946+47172</f>
-        <v>1900272</v>
+        <f>597309+190172+14984</f>
+        <v>802465</v>
       </c>
       <c r="U13" s="4">
         <f t="shared" si="3"/>
-        <v>8.5137464133333332</v>
+        <v>3.595266106944444</v>
       </c>
       <c r="V13" s="4">
         <f t="shared" si="0"/>
-        <v>10.151244420152912</v>
+        <v>13.883032009239738</v>
       </c>
       <c r="W13" s="4">
         <f t="shared" si="1"/>
-        <v>10.037452030841736</v>
+        <v>13.884159288295567</v>
       </c>
       <c r="X13" s="4">
         <f t="shared" si="2"/>
-        <v>0.23</v>
+        <v>0.25600000000000001</v>
       </c>
       <c r="Z13" t="s">
         <v>35</v>
       </c>
-      <c r="AB13" s="3"/>
-      <c r="AC13" s="3"/>
-      <c r="AD13" s="4"/>
-      <c r="AE13" s="4"/>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>27</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="D14">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E14">
-        <v>10222024</v>
+        <v>1112024</v>
       </c>
       <c r="F14" s="5">
-        <v>0.58680555555555558</v>
+        <v>0.51527777777777772</v>
       </c>
       <c r="G14" s="5">
-        <v>0.60833333333333328</v>
+        <v>0.5395833333333333</v>
       </c>
       <c r="H14" t="s">
         <v>28</v>
       </c>
       <c r="I14">
-        <v>29.93</v>
+        <v>23.27</v>
+      </c>
+      <c r="J14">
+        <v>0.01</v>
       </c>
       <c r="K14">
-        <v>24</v>
-      </c>
-      <c r="M14" s="2"/>
-      <c r="Q14" s="4"/>
+        <v>25</v>
+      </c>
       <c r="R14">
-        <v>0.73</v>
+        <v>0.40699999999999997</v>
       </c>
       <c r="S14">
-        <f>586040+374418+564372+8872+11168+28478</f>
-        <v>1573348</v>
+        <f>33714+510516+1144155</f>
+        <v>1688385</v>
       </c>
       <c r="U14" s="4">
         <f t="shared" si="3"/>
-        <v>7.0490360811111117</v>
+        <v>7.5644337958333328</v>
       </c>
       <c r="V14" s="4">
         <f t="shared" si="0"/>
-        <v>3.2313322723392002</v>
+        <v>4.1990693052370798</v>
       </c>
       <c r="W14" s="4">
         <f t="shared" si="1"/>
-        <v>3.3065983252733466</v>
+        <v>4.1994102626647241</v>
       </c>
       <c r="X14" s="4">
         <f t="shared" si="2"/>
-        <v>0.73</v>
+        <v>0.40699999999999997</v>
       </c>
       <c r="Z14" t="s">
         <v>35</v>
       </c>
-      <c r="AB14" s="3"/>
-      <c r="AC14" s="3"/>
-      <c r="AD14" s="4"/>
-      <c r="AE14" s="4"/>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>27</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15">
-        <v>3</v>
-      </c>
-      <c r="D15">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="E15">
-        <v>10222024</v>
+        <v>1112024</v>
       </c>
       <c r="F15" s="5">
-        <v>0.64722222222222225</v>
+        <v>0.50347222222222221</v>
       </c>
       <c r="G15" s="5">
-        <v>0.67222222222222228</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="H15" t="s">
         <v>28</v>
       </c>
       <c r="I15">
-        <v>30.13</v>
+        <v>29.17</v>
       </c>
       <c r="J15">
-        <v>1.4E-2</v>
-      </c>
-      <c r="K15" s="2">
-        <f>AVERAGE(K13:K14)</f>
-        <v>24.75</v>
+        <v>0.03</v>
+      </c>
+      <c r="K15">
+        <v>24</v>
       </c>
       <c r="R15">
-        <v>0.22</v>
+        <v>0.2</v>
       </c>
       <c r="S15">
-        <f>772708+721638+353300+141686+58053</f>
-        <v>2047385</v>
+        <f>1058307+519189+32007</f>
+        <v>1609503</v>
       </c>
       <c r="U15" s="4">
         <f t="shared" si="3"/>
-        <v>9.1728535180555557</v>
+        <v>7.2110205241666669</v>
       </c>
       <c r="V15" s="4">
         <f t="shared" si="0"/>
-        <v>8.2946771619206139</v>
+        <v>11.236658875983668</v>
       </c>
       <c r="W15" s="4">
         <f t="shared" si="1"/>
-        <v>8.3428226636098692</v>
+        <v>11.498389608227583</v>
       </c>
       <c r="X15" s="4">
         <f t="shared" si="2"/>
-        <v>0.22</v>
+        <v>0.2</v>
       </c>
       <c r="Z15" t="s">
         <v>35</v>
@@ -2727,779 +3766,902 @@
         <v>2</v>
       </c>
       <c r="C16">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E16">
-        <v>10232024</v>
+        <v>10222024</v>
       </c>
       <c r="F16" s="5">
-        <v>0.3888888888888889</v>
+        <v>0.48958333333333331</v>
       </c>
       <c r="G16" s="5">
-        <v>0.40694444444444444</v>
+        <v>0.46458333333333335</v>
       </c>
       <c r="H16" t="s">
         <v>28</v>
       </c>
       <c r="I16">
+        <v>35.78</v>
+      </c>
+      <c r="J16">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="K16" s="2">
+        <v>25.5</v>
+      </c>
+      <c r="M16" s="2"/>
+      <c r="Q16" s="4"/>
+      <c r="R16">
+        <v>0.23</v>
+      </c>
+      <c r="S16">
+        <f>758232+749922+344946+47172</f>
+        <v>1900272</v>
+      </c>
+      <c r="U16" s="4">
+        <f t="shared" si="3"/>
+        <v>8.5137464133333332</v>
+      </c>
+      <c r="V16" s="4">
+        <f t="shared" si="0"/>
+        <v>10.151244420152912</v>
+      </c>
+      <c r="W16" s="4">
+        <f t="shared" si="1"/>
+        <v>10.037452030841736</v>
+      </c>
+      <c r="X16" s="4">
+        <f t="shared" si="2"/>
+        <v>0.23</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB16" s="3"/>
+      <c r="AC16" s="3"/>
+      <c r="AD16" s="4"/>
+      <c r="AE16" s="4"/>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>10222024</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0.58680555555555558</v>
+      </c>
+      <c r="G17" s="5">
+        <v>0.60833333333333328</v>
+      </c>
+      <c r="H17" t="s">
+        <v>28</v>
+      </c>
+      <c r="I17">
+        <v>29.93</v>
+      </c>
+      <c r="K17">
+        <v>24</v>
+      </c>
+      <c r="M17" s="2"/>
+      <c r="Q17" s="4"/>
+      <c r="R17">
+        <v>0.73</v>
+      </c>
+      <c r="S17">
+        <f>586040+374418+564372+8872+11168+28478</f>
+        <v>1573348</v>
+      </c>
+      <c r="U17" s="4">
+        <f t="shared" si="3"/>
+        <v>7.0490360811111117</v>
+      </c>
+      <c r="V17" s="4">
+        <f t="shared" si="0"/>
+        <v>3.2313322723392002</v>
+      </c>
+      <c r="W17" s="4">
+        <f t="shared" si="1"/>
+        <v>3.3065983252733466</v>
+      </c>
+      <c r="X17" s="4">
+        <f t="shared" si="2"/>
+        <v>0.73</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB17" s="3"/>
+      <c r="AC17" s="3"/>
+      <c r="AD17" s="4"/>
+      <c r="AE17" s="4"/>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>10222024</v>
+      </c>
+      <c r="F18" s="5">
+        <v>0.64722222222222225</v>
+      </c>
+      <c r="G18" s="5">
+        <v>0.67222222222222228</v>
+      </c>
+      <c r="H18" t="s">
+        <v>28</v>
+      </c>
+      <c r="I18">
+        <v>30.13</v>
+      </c>
+      <c r="J18">
+        <v>1.4E-2</v>
+      </c>
+      <c r="K18" s="2">
+        <f>AVERAGE(K16:K17)</f>
+        <v>24.75</v>
+      </c>
+      <c r="R18">
+        <v>0.22</v>
+      </c>
+      <c r="S18">
+        <f>772708+721638+353300+141686+58053</f>
+        <v>2047385</v>
+      </c>
+      <c r="U18" s="4">
+        <f t="shared" si="3"/>
+        <v>9.1728535180555557</v>
+      </c>
+      <c r="V18" s="4">
+        <f t="shared" si="0"/>
+        <v>8.2946771619206139</v>
+      </c>
+      <c r="W18" s="4">
+        <f t="shared" si="1"/>
+        <v>8.3428226636098692</v>
+      </c>
+      <c r="X18" s="4">
+        <f t="shared" si="2"/>
+        <v>0.22</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>10232024</v>
+      </c>
+      <c r="F19" s="5">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="G19" s="5">
+        <v>0.40694444444444444</v>
+      </c>
+      <c r="H19" t="s">
+        <v>28</v>
+      </c>
+      <c r="I19">
         <v>31.36</v>
       </c>
-      <c r="J16">
+      <c r="J19">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="K16">
+      <c r="K19">
         <v>25</v>
       </c>
-      <c r="R16">
+      <c r="R19">
         <v>0.28000000000000003</v>
       </c>
-      <c r="S16">
+      <c r="S19">
         <f>640266+195606+138232+111298</f>
         <v>1085402</v>
       </c>
-      <c r="U16" s="4">
+      <c r="U19" s="4">
         <f t="shared" si="3"/>
         <v>4.8629024605555555</v>
       </c>
-      <c r="V16" s="4">
+      <c r="V19" s="4">
         <f t="shared" si="0"/>
         <v>12.795284858564431</v>
       </c>
-      <c r="W16" s="4">
+      <c r="W19" s="4">
         <f t="shared" si="1"/>
         <v>12.796323814364923</v>
       </c>
-      <c r="X16" s="4">
+      <c r="X19" s="4">
         <f t="shared" si="2"/>
         <v>0.28000000000000003</v>
       </c>
-      <c r="Z16" t="s">
+      <c r="Z19" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>27</v>
       </c>
-      <c r="B17">
+      <c r="B20">
         <v>2</v>
       </c>
-      <c r="C17">
+      <c r="C20">
         <v>5</v>
       </c>
-      <c r="D17">
+      <c r="D20">
         <v>2</v>
       </c>
-      <c r="E17">
+      <c r="E20">
         <v>10232024</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F20" s="5">
         <v>0.41388888888888886</v>
       </c>
-      <c r="G17" s="5">
+      <c r="G20" s="5">
         <v>0.44583333333333336</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H20" t="s">
         <v>28</v>
       </c>
-      <c r="I17">
+      <c r="I20">
         <v>21.26</v>
       </c>
-      <c r="J17">
+      <c r="J20">
         <v>0.03</v>
       </c>
-      <c r="K17">
+      <c r="K20">
         <v>25</v>
       </c>
-      <c r="R17">
+      <c r="R20">
         <v>1.96</v>
       </c>
-      <c r="S17">
+      <c r="S20">
         <f>1010963+603075+70608+42000</f>
         <v>1726646</v>
       </c>
-      <c r="U17" s="4">
+      <c r="U20" s="4">
         <f t="shared" si="3"/>
         <v>7.7358537038888882</v>
       </c>
-      <c r="V17" s="4">
+      <c r="V20" s="4">
         <f t="shared" si="0"/>
         <v>0.77898023000051075</v>
       </c>
-      <c r="W17" s="4">
+      <c r="W20" s="4">
         <f t="shared" si="1"/>
         <v>0.77904348189660955</v>
       </c>
-      <c r="X17" s="4">
+      <c r="X20" s="4">
         <f t="shared" si="2"/>
         <v>1.96</v>
       </c>
-      <c r="Z17" t="s">
+      <c r="Z20" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>27</v>
       </c>
-      <c r="B18">
+      <c r="B21">
         <v>2</v>
       </c>
-      <c r="C18">
+      <c r="C21">
         <v>6</v>
       </c>
-      <c r="D18">
+      <c r="D21">
         <v>2</v>
       </c>
-      <c r="E18">
+      <c r="E21">
         <v>10232024</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F21" s="5">
         <v>0.45416666666666666</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G21" s="5">
         <v>0.50138888888888888</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H21" t="s">
         <v>28</v>
       </c>
-      <c r="I18">
+      <c r="I21">
         <v>32.92</v>
       </c>
-      <c r="J18">
+      <c r="J21">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="K18">
+      <c r="K21">
         <v>25</v>
       </c>
-      <c r="R18">
+      <c r="R21">
         <v>0.06</v>
       </c>
-      <c r="S18">
+      <c r="S21">
         <f>959907+712944+315399+25575</f>
         <v>2013825</v>
       </c>
-      <c r="U18" s="4">
+      <c r="U21" s="4">
         <f t="shared" si="3"/>
         <v>9.0224953958333334</v>
       </c>
-      <c r="V18" s="4">
+      <c r="V21" s="4">
         <f t="shared" si="0"/>
         <v>33.783870364243242</v>
       </c>
-      <c r="W18" s="4">
+      <c r="W21" s="4">
         <f t="shared" si="1"/>
         <v>33.786613558198361</v>
       </c>
-      <c r="X18" s="4">
+      <c r="X21" s="4">
         <f t="shared" si="2"/>
         <v>0.06</v>
       </c>
-      <c r="Z18" t="s">
+      <c r="Z21" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>27</v>
       </c>
-      <c r="B19">
+      <c r="B22">
         <v>2</v>
       </c>
-      <c r="C19">
+      <c r="C22">
         <v>7</v>
       </c>
-      <c r="D19">
+      <c r="D22">
         <v>1</v>
       </c>
-      <c r="E19">
+      <c r="E22">
         <v>10292024</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F22" s="5">
         <v>0.36458333333333331</v>
       </c>
-      <c r="G19" s="5">
+      <c r="G22" s="5">
         <v>0.38541666666666669</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H22" t="s">
         <v>28</v>
       </c>
-      <c r="I19">
+      <c r="I22">
         <v>14.53</v>
       </c>
-      <c r="J19">
+      <c r="J22">
         <v>0.02</v>
       </c>
-      <c r="K19">
+      <c r="K22">
         <v>25</v>
       </c>
-      <c r="R19">
+      <c r="R22">
         <v>0.39400000000000002</v>
       </c>
-      <c r="S19">
+      <c r="S22">
         <f>406101+245400+54438</f>
         <v>705939</v>
       </c>
-      <c r="U19" s="4">
+      <c r="U22" s="4">
         <f t="shared" si="3"/>
         <v>3.1628028141666666</v>
       </c>
-      <c r="V19" s="4">
+      <c r="V22" s="4">
         <f t="shared" si="0"/>
         <v>6.4777587678543345</v>
       </c>
-      <c r="W19" s="4">
+      <c r="W22" s="4">
         <f t="shared" si="1"/>
         <v>6.4782847510677168</v>
       </c>
-      <c r="X19" s="4">
+      <c r="X22" s="4">
         <f t="shared" si="2"/>
         <v>0.39400000000000002</v>
       </c>
-      <c r="Z19" t="s">
+      <c r="Z22" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>27</v>
       </c>
-      <c r="B20">
+      <c r="B23">
         <v>2</v>
       </c>
-      <c r="C20">
+      <c r="C23">
         <v>8</v>
       </c>
-      <c r="D20">
+      <c r="D23">
         <v>1</v>
       </c>
-      <c r="E20">
+      <c r="E23">
         <v>10292024</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F23" s="5">
         <v>0.63472222222222219</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G23" s="5">
         <v>0.6645833333333333</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H23" t="s">
         <v>28</v>
       </c>
-      <c r="I20">
+      <c r="I23">
         <v>29.16</v>
       </c>
-      <c r="J20">
+      <c r="J23">
         <v>0.03</v>
       </c>
-      <c r="K20">
+      <c r="K23">
         <v>25</v>
       </c>
-      <c r="R20">
+      <c r="R23">
         <v>0.05</v>
       </c>
-      <c r="S20">
+      <c r="S23">
         <f>679974+285186+174309+63108</f>
         <v>1202577</v>
       </c>
-      <c r="U20" s="4">
+      <c r="U23" s="4">
         <f t="shared" si="3"/>
         <v>5.3878790091666673</v>
       </c>
-      <c r="V20" s="4">
+      <c r="V23" s="4">
         <f t="shared" si="0"/>
         <v>60.134980657279534</v>
       </c>
-      <c r="W20" s="4">
-        <f t="shared" si="1"/>
-        <v>60.139863517462565</v>
-      </c>
-      <c r="X20" s="4">
+      <c r="W23" s="4"/>
+      <c r="X23" s="4">
         <f t="shared" si="2"/>
         <v>0.05</v>
       </c>
-      <c r="Z20" t="s">
+      <c r="Z23" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>27</v>
       </c>
-      <c r="B21">
+      <c r="B24">
         <v>2</v>
       </c>
-      <c r="C21">
+      <c r="C24">
         <v>9</v>
       </c>
-      <c r="D21">
+      <c r="D24">
         <v>1</v>
       </c>
-      <c r="E21">
+      <c r="E24">
         <v>10292024</v>
       </c>
-      <c r="F21" s="5">
+      <c r="F24" s="5">
         <v>0.68055555555555558</v>
       </c>
-      <c r="G21" s="5">
+      <c r="G24" s="5">
         <v>0.70416666666666672</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H24" t="s">
         <v>28</v>
       </c>
-      <c r="I21">
+      <c r="I24">
         <v>9.5</v>
       </c>
-      <c r="J21">
+      <c r="J24">
         <v>0.05</v>
       </c>
-      <c r="K21">
+      <c r="K24">
         <v>24</v>
       </c>
-      <c r="R21" s="8">
+      <c r="R24" s="8">
         <v>0.25800000000000001</v>
       </c>
-      <c r="S21">
+      <c r="S24">
         <f>664089+263538</f>
         <v>927627</v>
       </c>
-      <c r="U21" s="4">
+      <c r="U24" s="4">
         <f t="shared" si="3"/>
         <v>4.1560266341666665</v>
       </c>
-      <c r="V21" s="4">
+      <c r="V24" s="4">
         <f t="shared" si="0"/>
         <v>4.9221299128522844</v>
       </c>
-      <c r="W21" s="4">
-        <f t="shared" si="1"/>
+      <c r="W24" s="4">
+        <f>V24/(0.88862*(1/POWER(10,(1.3272*(20-K24)-0.001053*(K24-20)^2)/(K24+105))))</f>
         <v>5.0367789985377067</v>
       </c>
-      <c r="X21" s="4">
+      <c r="X24" s="4">
         <f t="shared" si="2"/>
         <v>0.25800000000000001</v>
       </c>
-      <c r="Z21" t="s">
+      <c r="Z24" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>27</v>
       </c>
-      <c r="B22">
+      <c r="B25">
         <v>2</v>
       </c>
-      <c r="C22">
+      <c r="C25">
         <v>10</v>
       </c>
-      <c r="D22">
+      <c r="D25">
         <v>2</v>
       </c>
-      <c r="E22">
+      <c r="E25">
         <v>31102024</v>
       </c>
-      <c r="F22" s="5">
+      <c r="F25" s="5">
         <v>0.41944444444444445</v>
       </c>
-      <c r="G22" s="5">
+      <c r="G25" s="5">
         <v>0.44097222222222221</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H25" t="s">
         <v>28</v>
       </c>
-      <c r="I22" s="9">
+      <c r="I25" s="9">
         <v>1</v>
       </c>
-      <c r="J22" s="9">
+      <c r="J25" s="9">
         <v>1.34</v>
       </c>
-      <c r="K22">
+      <c r="K25">
         <v>22</v>
       </c>
-      <c r="R22">
+      <c r="R25">
         <v>0.63500000000000001</v>
       </c>
-      <c r="S22">
+      <c r="S25">
         <f>841923+510489+93468+76281</f>
         <v>1522161</v>
       </c>
-      <c r="U22" s="4">
+      <c r="U25" s="4">
         <f t="shared" si="3"/>
         <v>6.8197041025000003</v>
       </c>
-      <c r="V22" s="4">
+      <c r="V25" s="4">
         <f t="shared" si="0"/>
         <v>0.12828865087408184</v>
       </c>
-      <c r="W22" s="4">
-        <f t="shared" si="1"/>
+      <c r="W25" s="4">
+        <f>V25/(0.88862*(1/POWER(10,(1.3272*(20-K25)-0.001053*(K25-20)^2)/(K25+105))))</f>
         <v>0.13757458189717575</v>
       </c>
-      <c r="X22" s="4">
+      <c r="X25" s="4">
         <f t="shared" si="2"/>
         <v>0.63500000000000001</v>
       </c>
-      <c r="Z22" t="s">
+      <c r="Z25" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>27</v>
       </c>
-      <c r="B23">
+      <c r="B26">
         <v>2</v>
       </c>
-      <c r="C23">
+      <c r="C26">
         <v>11</v>
       </c>
-      <c r="D23">
+      <c r="D26">
         <v>1</v>
       </c>
-      <c r="E23">
+      <c r="E26">
         <v>31102024</v>
       </c>
-      <c r="F23" s="5">
+      <c r="F26" s="5">
         <v>0.43055555555555558</v>
       </c>
-      <c r="G23" s="5">
+      <c r="G26" s="5">
         <v>0.46388888888888891</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H26" t="s">
         <v>28</v>
       </c>
-      <c r="I23">
+      <c r="I26">
         <v>7.23</v>
       </c>
-      <c r="J23" s="9">
+      <c r="J26" s="9">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="K23">
+      <c r="K26">
         <v>22</v>
       </c>
-      <c r="R23">
+      <c r="R26">
         <v>0.89</v>
       </c>
-      <c r="S23">
+      <c r="S26">
         <f>336668+191234+97488+12270</f>
         <v>637660</v>
       </c>
-      <c r="U23" s="4">
+      <c r="U26" s="4">
         <f t="shared" si="3"/>
         <v>2.8568939277777776</v>
       </c>
-      <c r="V23" s="4">
+      <c r="V26" s="4">
         <f t="shared" si="0"/>
         <v>1.5797256490172571</v>
       </c>
-      <c r="W23" s="4">
-        <f t="shared" si="1"/>
+      <c r="W26" s="4">
+        <f>V26/(0.88862*(1/POWER(10,(1.3272*(20-K26)-0.001053*(K26-20)^2)/(K26+105))))</f>
         <v>1.694071098222929</v>
       </c>
-      <c r="X23" s="4">
+      <c r="X26" s="4">
         <f t="shared" si="2"/>
         <v>0.89</v>
       </c>
-      <c r="Z23" t="s">
+      <c r="Z26" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>27</v>
       </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24">
-        <v>11</v>
-      </c>
-      <c r="E24">
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>12</v>
+      </c>
+      <c r="E27">
         <v>1112024</v>
       </c>
-      <c r="F24" s="5">
-        <v>0.4777777777777778</v>
-      </c>
-      <c r="G24" s="5">
-        <v>0.49444444444444446</v>
-      </c>
-      <c r="H24" t="s">
+      <c r="F27" s="5">
+        <v>0.4597222222222222</v>
+      </c>
+      <c r="G27" s="5">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="H27" t="s">
         <v>28</v>
       </c>
-      <c r="I24">
-        <v>23</v>
-      </c>
-      <c r="J24">
-        <v>0.05</v>
-      </c>
-      <c r="K24">
+      <c r="I27">
+        <v>32.57</v>
+      </c>
+      <c r="J27">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="K27">
         <v>25</v>
       </c>
-      <c r="R24">
-        <v>0.25600000000000001</v>
-      </c>
-      <c r="S24">
-        <f>597309+190172+14984</f>
-        <v>802465</v>
-      </c>
-      <c r="U24" s="4">
-        <f t="shared" ref="U24:U27" si="4">S24/(1200^2)*2.54^2</f>
-        <v>3.595266106944444</v>
-      </c>
-      <c r="V24" s="4">
-        <f t="shared" ref="V24:V27" si="5">I24*0.000001/18*1000/R24/(U24/10000)</f>
-        <v>13.883032009239738</v>
-      </c>
-      <c r="W24" s="4">
-        <f t="shared" ref="W24:W27" si="6">V24/(0.88862*(1/POWER(10,(1.3272*(20-K24)-0.001053*(K24-20)^2)/(K24+105))))</f>
-        <v>13.884159288295567</v>
-      </c>
-      <c r="X24" s="4">
-        <f t="shared" ref="X24:X27" si="7">MAX(Q24:R24)</f>
-        <v>0.25600000000000001</v>
-      </c>
-      <c r="Z24" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25">
-        <v>2</v>
-      </c>
-      <c r="C25">
-        <v>12</v>
-      </c>
-      <c r="E25">
-        <v>1112024</v>
-      </c>
-      <c r="F25" s="5">
-        <v>0.4597222222222222</v>
-      </c>
-      <c r="G25" s="5">
-        <v>0.47499999999999998</v>
-      </c>
-      <c r="H25" t="s">
-        <v>28</v>
-      </c>
-      <c r="I25">
-        <v>32.57</v>
-      </c>
-      <c r="J25">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="K25">
-        <v>25</v>
-      </c>
-      <c r="R25">
+      <c r="R27">
         <v>1.4770000000000001</v>
       </c>
-      <c r="S25">
+      <c r="S27">
         <f>693572+299597+149838+15127</f>
         <v>1158134</v>
       </c>
-      <c r="U25" s="4">
-        <f t="shared" si="4"/>
+      <c r="U27" s="4">
+        <f t="shared" si="3"/>
         <v>5.1887620238888887</v>
       </c>
-      <c r="V25" s="4">
-        <f t="shared" si="5"/>
+      <c r="V27" s="4">
+        <f t="shared" si="0"/>
         <v>2.3610272816336555</v>
       </c>
-      <c r="W25" s="4">
-        <f t="shared" si="6"/>
+      <c r="W27" s="4">
+        <f>V27/(0.88862*(1/POWER(10,(1.3272*(20-K27)-0.001053*(K27-20)^2)/(K27+105))))</f>
         <v>2.3612189931130394</v>
       </c>
-      <c r="X25" s="4">
-        <f t="shared" si="7"/>
+      <c r="X27" s="4">
+        <f t="shared" si="2"/>
         <v>1.4770000000000001</v>
       </c>
-      <c r="Z25" t="s">
+      <c r="Z27" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>27</v>
       </c>
-      <c r="B26">
+      <c r="B28">
         <v>2</v>
       </c>
-      <c r="C26">
+      <c r="C28">
         <v>13</v>
       </c>
-      <c r="E26">
+      <c r="E28">
         <v>1112024</v>
       </c>
-      <c r="F26" s="5">
+      <c r="F28" s="5">
         <v>0.44930555555555557</v>
       </c>
-      <c r="G26" s="5">
+      <c r="G28" s="5">
         <v>0.47361111111111109</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H28" t="s">
         <v>28</v>
       </c>
-      <c r="I26">
+      <c r="I28">
         <v>27.9</v>
       </c>
-      <c r="J26">
+      <c r="J28">
         <v>0.02</v>
       </c>
-      <c r="K26">
+      <c r="K28">
         <v>24</v>
       </c>
-      <c r="R26">
+      <c r="R28">
         <v>0.39300000000000002</v>
       </c>
-      <c r="S26">
+      <c r="S28">
         <f>1201677+733659+346472+23738</f>
         <v>2305546</v>
       </c>
-      <c r="U26" s="4">
-        <f t="shared" si="4"/>
+      <c r="U28" s="4">
+        <f t="shared" si="3"/>
         <v>10.329486509444443</v>
       </c>
-      <c r="V26" s="4">
-        <f t="shared" si="5"/>
+      <c r="V28" s="4">
+        <f t="shared" si="0"/>
         <v>3.8182153126663207</v>
       </c>
-      <c r="W26" s="4">
-        <f t="shared" si="6"/>
+      <c r="W28" s="4">
+        <f>V28/(0.88862*(1/POWER(10,(1.3272*(20-K28)-0.001053*(K28-20)^2)/(K28+105))))</f>
         <v>3.9071513834929439</v>
       </c>
-      <c r="X26" s="4">
-        <f t="shared" si="7"/>
+      <c r="X28" s="4">
+        <f t="shared" si="2"/>
         <v>0.39300000000000002</v>
-      </c>
-      <c r="Z26" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27">
-        <v>12</v>
-      </c>
-      <c r="E27">
-        <v>1112024</v>
-      </c>
-      <c r="F27" s="5">
-        <v>0.51527777777777772</v>
-      </c>
-      <c r="G27" s="5">
-        <v>0.5395833333333333</v>
-      </c>
-      <c r="H27" t="s">
-        <v>28</v>
-      </c>
-      <c r="I27">
-        <v>23.27</v>
-      </c>
-      <c r="J27">
-        <v>0.01</v>
-      </c>
-      <c r="K27">
-        <v>25</v>
-      </c>
-      <c r="R27">
-        <v>0.40699999999999997</v>
-      </c>
-      <c r="S27">
-        <f>33714+510516+1144155</f>
-        <v>1688385</v>
-      </c>
-      <c r="U27" s="4">
-        <f t="shared" si="4"/>
-        <v>7.5644337958333328</v>
-      </c>
-      <c r="V27" s="4">
-        <f t="shared" si="5"/>
-        <v>4.1990693052370798</v>
-      </c>
-      <c r="W27" s="4">
-        <f t="shared" si="6"/>
-        <v>4.1994102626647241</v>
-      </c>
-      <c r="X27" s="4">
-        <f t="shared" si="7"/>
-        <v>0.40699999999999997</v>
-      </c>
-      <c r="Z27" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>27</v>
-      </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28">
-        <v>13</v>
-      </c>
-      <c r="E28">
-        <v>1112024</v>
-      </c>
-      <c r="F28" s="5">
-        <v>0.50347222222222221</v>
-      </c>
-      <c r="G28" s="5">
-        <v>0.52083333333333337</v>
-      </c>
-      <c r="H28" t="s">
-        <v>28</v>
-      </c>
-      <c r="I28">
-        <v>29.17</v>
-      </c>
-      <c r="J28">
-        <v>0.03</v>
-      </c>
-      <c r="K28">
-        <v>24</v>
-      </c>
-      <c r="R28">
-        <v>0.2</v>
-      </c>
-      <c r="S28">
-        <f>1058307+519189+32007</f>
-        <v>1609503</v>
-      </c>
-      <c r="U28" s="4">
-        <f t="shared" ref="U28" si="8">S28/(1200^2)*2.54^2</f>
-        <v>7.2110205241666669</v>
-      </c>
-      <c r="V28" s="4">
-        <f t="shared" ref="V28" si="9">I28*0.000001/18*1000/R28/(U28/10000)</f>
-        <v>11.236658875983668</v>
-      </c>
-      <c r="W28" s="4">
-        <f t="shared" ref="W28" si="10">V28/(0.88862*(1/POWER(10,(1.3272*(20-K28)-0.001053*(K28-20)^2)/(K28+105))))</f>
-        <v>11.498389608227583</v>
-      </c>
-      <c r="X28" s="4">
-        <f t="shared" ref="X28" si="11">MAX(Q28:R28)</f>
-        <v>0.2</v>
       </c>
       <c r="Z28" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>14</v>
+      </c>
+      <c r="E29">
+        <v>11052024</v>
+      </c>
+      <c r="F29" s="5">
+        <v>0.40902777777777777</v>
+      </c>
+      <c r="G29" s="5">
+        <v>0.42569444444444443</v>
+      </c>
+      <c r="I29">
+        <v>41.2</v>
+      </c>
+      <c r="J29">
+        <v>0.05</v>
+      </c>
+      <c r="K29">
+        <v>26</v>
+      </c>
+      <c r="R29" s="10">
+        <v>1.7569999999999999</v>
+      </c>
+      <c r="S29">
+        <f>970585+271027+38180</f>
+        <v>1279792</v>
+      </c>
+      <c r="U29" s="4">
+        <f t="shared" ref="U29:U30" si="4">S29/(1200^2)*2.54^2</f>
+        <v>5.7338236577777781</v>
+      </c>
+      <c r="V29" s="4">
+        <f t="shared" ref="V29:V30" si="5">I29*0.000001/18*1000/R29/(U29/10000)</f>
+        <v>2.2720015181271536</v>
+      </c>
+      <c r="W29" s="4">
+        <f t="shared" ref="W29:W30" si="6">V29/(0.88862*(1/POWER(10,(1.3272*(20-K29)-0.001053*(K29-20)^2)/(K29+105))))</f>
+        <v>2.2213417198360363</v>
+      </c>
+      <c r="X29" s="4">
+        <f t="shared" si="2"/>
+        <v>1.7569999999999999</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30">
+        <v>14</v>
+      </c>
+      <c r="E30">
+        <v>11052024</v>
+      </c>
+      <c r="F30" s="5">
+        <v>0.40486111111111112</v>
+      </c>
+      <c r="G30" s="5">
+        <v>0.42569444444444443</v>
+      </c>
+      <c r="I30">
+        <v>11.76</v>
+      </c>
+      <c r="J30">
+        <v>0.03</v>
+      </c>
+      <c r="K30">
+        <v>26</v>
+      </c>
+      <c r="R30">
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="S30">
+        <f>728773+107895+147482</f>
+        <v>984150</v>
+      </c>
+      <c r="U30" s="4">
+        <f t="shared" si="4"/>
+        <v>4.4092653750000004</v>
+      </c>
+      <c r="V30" s="4">
+        <f t="shared" si="5"/>
+        <v>1.7787854864376267</v>
+      </c>
+      <c r="W30" s="4">
+        <f t="shared" si="6"/>
+        <v>1.7391231388436081</v>
+      </c>
+      <c r="X30" s="4">
+        <f t="shared" si="2"/>
+        <v>0.83299999999999996</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:AE23" xr:uid="{E3FF746F-B21E-4AE2-A531-A971B17E5B05}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AE23">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AE28">
       <sortCondition ref="B1:B23"/>
     </sortState>
   </autoFilter>
@@ -3507,4 +4669,1496 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33064BB3-47FF-4DAF-9632-D6C75923AEEE}">
+  <dimension ref="A1:AE26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="S4" sqref="S4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="V1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="W1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="X1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="8">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8">
+        <v>1</v>
+      </c>
+      <c r="D2" s="8">
+        <v>2</v>
+      </c>
+      <c r="E2" s="8">
+        <v>10222024</v>
+      </c>
+      <c r="F2" s="11">
+        <v>0.50208333333333333</v>
+      </c>
+      <c r="G2" s="11">
+        <v>0.52152777777777781</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="8">
+        <v>25.26</v>
+      </c>
+      <c r="J2" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="K2" s="12">
+        <f>AVERAGE(K6,K7)</f>
+        <v>26</v>
+      </c>
+      <c r="M2" s="12"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="8">
+        <v>0.155</v>
+      </c>
+      <c r="S2" s="8">
+        <f>917270+813318+608426+406146</f>
+        <v>2745160</v>
+      </c>
+      <c r="U2" s="13">
+        <f>S2/(1200^2)*2.54^2</f>
+        <v>12.299079344444445</v>
+      </c>
+      <c r="V2" s="13">
+        <f>I2*0.000001/18*1000/R2/(U2/10000)</f>
+        <v>7.3613342814556653</v>
+      </c>
+      <c r="W2" s="13">
+        <f>V2/(0.88862*(1/POWER(10,(1.3272*(20-K2)-0.001053*(K2-20)^2)/(K2+105))))</f>
+        <v>7.197195434330494</v>
+      </c>
+      <c r="X2" s="13">
+        <f>MAX(Q2:R2)</f>
+        <v>0.155</v>
+      </c>
+      <c r="Z2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB2" s="14"/>
+      <c r="AC2" s="14"/>
+      <c r="AD2" s="13"/>
+      <c r="AE2" s="13"/>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>11052024</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0.43402777777777779</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0.45</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3">
+        <v>76.03</v>
+      </c>
+      <c r="J3">
+        <v>0.04</v>
+      </c>
+      <c r="K3">
+        <v>28</v>
+      </c>
+      <c r="R3">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="S3">
+        <f>3742239+1736196+274185</f>
+        <v>5752620</v>
+      </c>
+      <c r="U3" s="4">
+        <f>S3/(1200^2)*2.54^2</f>
+        <v>25.773335549999999</v>
+      </c>
+      <c r="V3" s="4">
+        <f>I3*0.000001/18*1000/R3/(U3/10000)</f>
+        <v>1.7736580166117932</v>
+      </c>
+      <c r="W3" s="4">
+        <f>V3/(0.88862*(1/POWER(10,(1.3272*(20-K3)-0.001053*(K3-20)^2)/(K3+105))))</f>
+        <v>1.6588820843428438</v>
+      </c>
+      <c r="X3" s="4">
+        <f>MAX(Q3:R3)</f>
+        <v>0.92400000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>11052024</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0.44583333333333336</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0.4597222222222222</v>
+      </c>
+      <c r="I4">
+        <v>151.93</v>
+      </c>
+      <c r="J4">
+        <v>0.02</v>
+      </c>
+      <c r="K4">
+        <v>25</v>
+      </c>
+      <c r="R4">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="S4">
+        <f>2819618+740109+62919</f>
+        <v>3622646</v>
+      </c>
+      <c r="U4" s="4">
+        <f t="shared" ref="U4:U17" si="0">S4/(1200^2)*2.54^2</f>
+        <v>16.230460370555555</v>
+      </c>
+      <c r="V4" s="4">
+        <f t="shared" ref="V4:V17" si="1">I4*0.000001/18*1000/R4/(U4/10000)</f>
+        <v>75.368713712779083</v>
+      </c>
+      <c r="W4" s="4">
+        <f t="shared" ref="W4:W17" si="2">V4/(0.88862*(1/POWER(10,(1.3272*(20-K4)-0.001053*(K4-20)^2)/(K4+105))))</f>
+        <v>75.374833526691248</v>
+      </c>
+      <c r="X4" s="4">
+        <f t="shared" ref="X4:X17" si="3">MAX(Q4:R4)</f>
+        <v>6.9000000000000006E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>11052024</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0.47083333333333333</v>
+      </c>
+      <c r="I5">
+        <v>57.03</v>
+      </c>
+      <c r="J5">
+        <v>0.03</v>
+      </c>
+      <c r="K5">
+        <v>29</v>
+      </c>
+      <c r="R5">
+        <v>1.075</v>
+      </c>
+      <c r="S5">
+        <f>4925019+4340568+566136+170205</f>
+        <v>10001928</v>
+      </c>
+      <c r="U5" s="4">
+        <f t="shared" si="0"/>
+        <v>44.811415753333328</v>
+      </c>
+      <c r="V5" s="4">
+        <f t="shared" si="1"/>
+        <v>0.65770892799480229</v>
+      </c>
+      <c r="W5" s="4">
+        <f t="shared" si="2"/>
+        <v>0.6019228638124352</v>
+      </c>
+      <c r="X5" s="4">
+        <f t="shared" si="3"/>
+        <v>1.075</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>11052024</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0.46875</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="I6">
+        <v>123.23</v>
+      </c>
+      <c r="J6">
+        <v>0.04</v>
+      </c>
+      <c r="K6">
+        <v>26</v>
+      </c>
+      <c r="R6">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="S6">
+        <f>2960525+1858284+185796</f>
+        <v>5004605</v>
+      </c>
+      <c r="U6" s="4">
+        <f t="shared" si="0"/>
+        <v>22.422020568055558</v>
+      </c>
+      <c r="V6" s="4">
+        <f t="shared" si="1"/>
+        <v>31.156102293259579</v>
+      </c>
+      <c r="W6" s="4">
+        <f t="shared" si="2"/>
+        <v>30.46140123557058</v>
+      </c>
+      <c r="X6" s="4">
+        <f t="shared" si="3"/>
+        <v>9.8000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>11052024</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0.50555555555555554</v>
+      </c>
+      <c r="G7" s="5">
+        <v>0.5180555555555556</v>
+      </c>
+      <c r="I7">
+        <v>164.5667</v>
+      </c>
+      <c r="J7">
+        <v>0.05</v>
+      </c>
+      <c r="K7">
+        <v>26</v>
+      </c>
+      <c r="R7">
+        <v>0.95899999999999996</v>
+      </c>
+      <c r="S7">
+        <f>4835739+3175523+449619</f>
+        <v>8460881</v>
+      </c>
+      <c r="U7" s="4">
+        <f t="shared" si="0"/>
+        <v>37.90709712472222</v>
+      </c>
+      <c r="V7" s="4">
+        <f t="shared" si="1"/>
+        <v>2.5149555880289221</v>
+      </c>
+      <c r="W7" s="4">
+        <f t="shared" si="2"/>
+        <v>2.458878537998741</v>
+      </c>
+      <c r="X7" s="4">
+        <f t="shared" si="3"/>
+        <v>0.95899999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>11052024</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0.49513888888888891</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0.5131944444444444</v>
+      </c>
+      <c r="I8">
+        <v>53.63</v>
+      </c>
+      <c r="J8">
+        <v>0.06</v>
+      </c>
+      <c r="K8">
+        <v>27</v>
+      </c>
+      <c r="R8">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="S8">
+        <f>4653196+1606899+337131</f>
+        <v>6597226</v>
+      </c>
+      <c r="U8" s="4">
+        <f t="shared" si="0"/>
+        <v>29.557405042777781</v>
+      </c>
+      <c r="V8" s="4">
+        <f t="shared" si="1"/>
+        <v>0.92478864980754472</v>
+      </c>
+      <c r="W8" s="4">
+        <f t="shared" si="2"/>
+        <v>0.88420649912393312</v>
+      </c>
+      <c r="X8" s="4">
+        <f t="shared" si="3"/>
+        <v>1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>11052024</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0.52430555555555558</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0.53680555555555554</v>
+      </c>
+      <c r="I9">
+        <v>224.1</v>
+      </c>
+      <c r="J9">
+        <v>0.03</v>
+      </c>
+      <c r="K9">
+        <v>27</v>
+      </c>
+      <c r="R9">
+        <v>0.27800000000000002</v>
+      </c>
+      <c r="S9">
+        <f>4626500+3749898+51222+51093+359223+219051</f>
+        <v>9056987</v>
+      </c>
+      <c r="U9" s="4">
+        <f t="shared" si="0"/>
+        <v>40.577817589722223</v>
+      </c>
+      <c r="V9" s="4">
+        <f t="shared" si="1"/>
+        <v>11.036614416940372</v>
+      </c>
+      <c r="W9" s="4">
+        <f t="shared" si="2"/>
+        <v>10.552298839107099</v>
+      </c>
+      <c r="X9" s="4">
+        <f t="shared" si="3"/>
+        <v>0.27800000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>11052024</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0.55694444444444446</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0.57222222222222219</v>
+      </c>
+      <c r="I10">
+        <v>164.23</v>
+      </c>
+      <c r="J10">
+        <v>0.03</v>
+      </c>
+      <c r="K10">
+        <v>23</v>
+      </c>
+      <c r="R10">
+        <v>0.76</v>
+      </c>
+      <c r="S10">
+        <f>3827186+2992989+427437+255441+200562</f>
+        <v>7703615</v>
+      </c>
+      <c r="U10" s="4">
+        <f t="shared" si="0"/>
+        <v>34.514335093055557</v>
+      </c>
+      <c r="V10" s="4">
+        <f t="shared" si="1"/>
+        <v>3.4782987783762378</v>
+      </c>
+      <c r="W10" s="4">
+        <f t="shared" si="2"/>
+        <v>3.6430951275139472</v>
+      </c>
+      <c r="X10" s="4">
+        <f t="shared" si="3"/>
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>11052024</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0.56597222222222221</v>
+      </c>
+      <c r="G11" s="5">
+        <v>0.57986111111111116</v>
+      </c>
+      <c r="I11">
+        <v>50.36</v>
+      </c>
+      <c r="J11">
+        <v>0.02</v>
+      </c>
+      <c r="K11">
+        <v>25</v>
+      </c>
+      <c r="R11">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="S11">
+        <f>5553959+2731359+102816+113724+387417</f>
+        <v>8889275</v>
+      </c>
+      <c r="U11" s="4">
+        <f t="shared" si="0"/>
+        <v>39.826421243055556</v>
+      </c>
+      <c r="V11" s="4">
+        <f t="shared" si="1"/>
+        <v>0.75945177352635507</v>
+      </c>
+      <c r="W11" s="4">
+        <f t="shared" si="2"/>
+        <v>0.75951343974434249</v>
+      </c>
+      <c r="X11" s="4">
+        <f t="shared" si="3"/>
+        <v>0.92500000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>11052024</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0.57638888888888884</v>
+      </c>
+      <c r="G12" s="5">
+        <v>0.59027777777777779</v>
+      </c>
+      <c r="I12">
+        <v>173.56</v>
+      </c>
+      <c r="J12">
+        <v>0.01</v>
+      </c>
+      <c r="K12">
+        <v>26</v>
+      </c>
+      <c r="R12">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="S12">
+        <f>3911688+2586837+234777</f>
+        <v>6733302</v>
+      </c>
+      <c r="U12" s="4">
+        <f t="shared" si="0"/>
+        <v>30.167063321666664</v>
+      </c>
+      <c r="V12" s="4">
+        <f t="shared" si="1"/>
+        <v>15.148221476871813</v>
+      </c>
+      <c r="W12" s="4">
+        <f t="shared" si="2"/>
+        <v>14.810455045659179</v>
+      </c>
+      <c r="X12" s="4">
+        <f t="shared" si="3"/>
+        <v>0.21099999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>11052024</v>
+      </c>
+      <c r="F13" s="5">
+        <v>0.58750000000000002</v>
+      </c>
+      <c r="G13" s="5">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="I13">
+        <v>156.56</v>
+      </c>
+      <c r="J13">
+        <v>0.04</v>
+      </c>
+      <c r="K13">
+        <v>25</v>
+      </c>
+      <c r="R13">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="S13">
+        <f>4606628+4315754+488439+348738</f>
+        <v>9759559</v>
+      </c>
+      <c r="U13" s="4">
+        <f t="shared" si="0"/>
+        <v>43.725535308611114</v>
+      </c>
+      <c r="V13" s="4">
+        <f t="shared" si="1"/>
+        <v>2.2501988972322793</v>
+      </c>
+      <c r="W13" s="4">
+        <f t="shared" si="2"/>
+        <v>2.2503816096316034</v>
+      </c>
+      <c r="X13" s="4">
+        <f t="shared" si="3"/>
+        <v>0.88400000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>11052024</v>
+      </c>
+      <c r="F14" s="5">
+        <v>0.59513888888888888</v>
+      </c>
+      <c r="G14" s="5">
+        <v>0.60902777777777772</v>
+      </c>
+      <c r="I14">
+        <v>132</v>
+      </c>
+      <c r="J14">
+        <v>0.02</v>
+      </c>
+      <c r="K14">
+        <v>26</v>
+      </c>
+      <c r="R14">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="S14">
+        <f>5509488+5131139+994746+337377</f>
+        <v>11972750</v>
+      </c>
+      <c r="U14" s="4">
+        <f t="shared" si="0"/>
+        <v>53.64124576388889</v>
+      </c>
+      <c r="V14" s="4">
+        <f t="shared" si="1"/>
+        <v>1.9870744194866772</v>
+      </c>
+      <c r="W14" s="4">
+        <f t="shared" si="2"/>
+        <v>1.942767763669117</v>
+      </c>
+      <c r="X14" s="4">
+        <f t="shared" si="3"/>
+        <v>0.68799999999999994</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>11052024</v>
+      </c>
+      <c r="F15" s="5">
+        <v>0.61250000000000004</v>
+      </c>
+      <c r="G15" s="5">
+        <v>0.63055555555555554</v>
+      </c>
+      <c r="I15">
+        <v>96.5</v>
+      </c>
+      <c r="J15">
+        <v>0.04</v>
+      </c>
+      <c r="K15">
+        <v>25</v>
+      </c>
+      <c r="R15">
+        <v>6.3E-2</v>
+      </c>
+      <c r="S15">
+        <f>3283770+1405266</f>
+        <v>4689036</v>
+      </c>
+      <c r="U15" s="4">
+        <f t="shared" si="0"/>
+        <v>21.00818379</v>
+      </c>
+      <c r="V15" s="4">
+        <f t="shared" si="1"/>
+        <v>40.506596198084964</v>
+      </c>
+      <c r="W15" s="4">
+        <f t="shared" si="2"/>
+        <v>40.509885266170855</v>
+      </c>
+      <c r="X15" s="4">
+        <f t="shared" si="3"/>
+        <v>6.3E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>11052024</v>
+      </c>
+      <c r="F16" s="5">
+        <v>0.61527777777777781</v>
+      </c>
+      <c r="G16" s="5">
+        <v>0.63263888888888886</v>
+      </c>
+      <c r="I16">
+        <v>58.93</v>
+      </c>
+      <c r="J16">
+        <v>0.04</v>
+      </c>
+      <c r="K16">
+        <v>25</v>
+      </c>
+      <c r="R16">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="S16">
+        <f>3146154+556854</f>
+        <v>3703008</v>
+      </c>
+      <c r="U16" s="4">
+        <f t="shared" si="0"/>
+        <v>16.590504453333335</v>
+      </c>
+      <c r="V16" s="4">
+        <f t="shared" si="1"/>
+        <v>29.453000301736257</v>
+      </c>
+      <c r="W16" s="4">
+        <f t="shared" si="2"/>
+        <v>29.455391836261956</v>
+      </c>
+      <c r="X16" s="4">
+        <f t="shared" si="3"/>
+        <v>6.7000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>11052024</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0.63611111111111107</v>
+      </c>
+      <c r="G17" s="5">
+        <v>0.65</v>
+      </c>
+      <c r="I17">
+        <v>79.3</v>
+      </c>
+      <c r="J17">
+        <v>0.01</v>
+      </c>
+      <c r="K17">
+        <v>25</v>
+      </c>
+      <c r="R17">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="S17">
+        <f>4107921+4268460+352713+688113</f>
+        <v>9417207</v>
+      </c>
+      <c r="U17" s="4">
+        <f t="shared" si="0"/>
+        <v>42.191703250833335</v>
+      </c>
+      <c r="V17" s="4">
+        <f t="shared" si="1"/>
+        <v>8.9245794993854837</v>
+      </c>
+      <c r="W17" s="4">
+        <f t="shared" si="2"/>
+        <v>8.9253041603633623</v>
+      </c>
+      <c r="X17" s="4">
+        <f t="shared" si="3"/>
+        <v>0.11700000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="9">
+        <v>3</v>
+      </c>
+      <c r="C18" s="9">
+        <v>7</v>
+      </c>
+      <c r="D18" s="9">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>11062024</v>
+      </c>
+      <c r="F18" s="5">
+        <v>0.45277777777777778</v>
+      </c>
+      <c r="G18" s="5">
+        <v>0.46944444444444444</v>
+      </c>
+      <c r="I18">
+        <v>81.93</v>
+      </c>
+      <c r="J18">
+        <v>0.03</v>
+      </c>
+      <c r="K18">
+        <v>26</v>
+      </c>
+      <c r="U18" s="4">
+        <f t="shared" ref="U18:U26" si="4">S18/(1200^2)*2.54^2</f>
+        <v>0</v>
+      </c>
+      <c r="V18" s="4" t="e">
+        <f t="shared" ref="V18:V26" si="5">I18*0.000001/18*1000/R18/(U18/10000)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W18" s="4" t="e">
+        <f t="shared" ref="W18:W26" si="6">V18/(0.88862*(1/POWER(10,(1.3272*(20-K18)-0.001053*(K18-20)^2)/(K18+105))))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X18" s="4">
+        <f t="shared" ref="X18:X26" si="7">MAX(Q18:R18)</f>
+        <v>0</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <v>6</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>11062024</v>
+      </c>
+      <c r="F19" s="5">
+        <v>0.44583333333333336</v>
+      </c>
+      <c r="G19" s="5">
+        <v>0.46041666666666664</v>
+      </c>
+      <c r="I19">
+        <v>93.93</v>
+      </c>
+      <c r="J19">
+        <v>0.05</v>
+      </c>
+      <c r="K19">
+        <v>27</v>
+      </c>
+      <c r="R19">
+        <v>1.0640000000000001</v>
+      </c>
+      <c r="S19">
+        <f>4488064+3975008+820142+388906+446306</f>
+        <v>10118426</v>
+      </c>
+      <c r="U19" s="4">
+        <f t="shared" si="4"/>
+        <v>45.333359153888885</v>
+      </c>
+      <c r="V19" s="4">
+        <f t="shared" si="5"/>
+        <v>1.0818630503213351</v>
+      </c>
+      <c r="W19" s="4">
+        <f t="shared" si="6"/>
+        <v>1.0343880631052735</v>
+      </c>
+      <c r="X19" s="4">
+        <f t="shared" si="7"/>
+        <v>1.0640000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>7</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>11062024</v>
+      </c>
+      <c r="F20" s="5">
+        <v>0.47291666666666665</v>
+      </c>
+      <c r="G20" s="5">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="I20">
+        <v>56</v>
+      </c>
+      <c r="J20">
+        <v>0.04</v>
+      </c>
+      <c r="K20">
+        <v>26</v>
+      </c>
+      <c r="R20">
+        <v>0.58299999999999996</v>
+      </c>
+      <c r="S20">
+        <f>3148502+973545+623022</f>
+        <v>4745069</v>
+      </c>
+      <c r="U20" s="4">
+        <f t="shared" si="4"/>
+        <v>21.259227194722225</v>
+      </c>
+      <c r="V20" s="4">
+        <f t="shared" si="5"/>
+        <v>2.5101489560251102</v>
+      </c>
+      <c r="W20" s="4">
+        <f t="shared" si="6"/>
+        <v>2.4541790815429341</v>
+      </c>
+      <c r="X20" s="4">
+        <f t="shared" si="7"/>
+        <v>0.58299999999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>6</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <v>11062024</v>
+      </c>
+      <c r="F21" s="5">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="G21" s="5">
+        <v>0.49652777777777779</v>
+      </c>
+      <c r="I21">
+        <v>50.66</v>
+      </c>
+      <c r="J21">
+        <v>0.04</v>
+      </c>
+      <c r="K21">
+        <v>27</v>
+      </c>
+      <c r="R21">
+        <v>1.012</v>
+      </c>
+      <c r="S21">
+        <f>4433450+4827611+725994+513558</f>
+        <v>10500613</v>
+      </c>
+      <c r="U21" s="4">
+        <f t="shared" si="4"/>
+        <v>47.045663076944443</v>
+      </c>
+      <c r="V21" s="4">
+        <f t="shared" si="5"/>
+        <v>0.5911430307339689</v>
+      </c>
+      <c r="W21" s="4">
+        <f t="shared" si="6"/>
+        <v>0.56520212461038577</v>
+      </c>
+      <c r="X21" s="4">
+        <f t="shared" si="7"/>
+        <v>1.012</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>8</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>11062024</v>
+      </c>
+      <c r="F22" s="5">
+        <v>0.49652777777777779</v>
+      </c>
+      <c r="G22" s="5">
+        <v>0.51111111111111107</v>
+      </c>
+      <c r="I22">
+        <v>44.1</v>
+      </c>
+      <c r="J22">
+        <v>0.04</v>
+      </c>
+      <c r="K22">
+        <v>27</v>
+      </c>
+      <c r="R22">
+        <v>1.129</v>
+      </c>
+      <c r="S22">
+        <f>4187364+1348485+875083</f>
+        <v>6410932</v>
+      </c>
+      <c r="U22" s="4">
+        <f t="shared" si="4"/>
+        <v>28.722756174444445</v>
+      </c>
+      <c r="V22" s="4">
+        <f t="shared" si="5"/>
+        <v>0.75552011394444563</v>
+      </c>
+      <c r="W22" s="4">
+        <f t="shared" si="6"/>
+        <v>0.72236591042456721</v>
+      </c>
+      <c r="X22" s="4">
+        <f t="shared" si="7"/>
+        <v>1.129</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>6</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23">
+        <v>11062024</v>
+      </c>
+      <c r="F23" s="5">
+        <v>0.50208333333333333</v>
+      </c>
+      <c r="G23" s="5">
+        <v>0.51597222222222228</v>
+      </c>
+      <c r="I23">
+        <v>180.83</v>
+      </c>
+      <c r="J23">
+        <v>0.04</v>
+      </c>
+      <c r="K23">
+        <v>27</v>
+      </c>
+      <c r="R23">
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="S23">
+        <f>4228048+3603816+468196+357866</f>
+        <v>8657926</v>
+      </c>
+      <c r="U23" s="4">
+        <f t="shared" si="4"/>
+        <v>38.789913459444442</v>
+      </c>
+      <c r="V23" s="4">
+        <f t="shared" si="5"/>
+        <v>2.9975430153497418</v>
+      </c>
+      <c r="W23" s="4">
+        <f t="shared" si="6"/>
+        <v>2.8660029684916339</v>
+      </c>
+      <c r="X23" s="4">
+        <f t="shared" si="7"/>
+        <v>0.86399999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>7</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>11062024</v>
+      </c>
+      <c r="F24" s="5">
+        <v>0.51875000000000004</v>
+      </c>
+      <c r="G24" s="5">
+        <v>0.53125</v>
+      </c>
+      <c r="I24">
+        <v>96.1</v>
+      </c>
+      <c r="J24">
+        <v>0.04</v>
+      </c>
+      <c r="K24">
+        <v>26</v>
+      </c>
+      <c r="R24">
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="S24">
+        <f>3786410+4326989+1369523+275086</f>
+        <v>9758008</v>
+      </c>
+      <c r="U24" s="4">
+        <f t="shared" si="4"/>
+        <v>43.718586397777777</v>
+      </c>
+      <c r="V24" s="4">
+        <f t="shared" si="5"/>
+        <v>1.306090169622862</v>
+      </c>
+      <c r="W24" s="4">
+        <f t="shared" si="6"/>
+        <v>1.2769677134910338</v>
+      </c>
+      <c r="X24" s="4">
+        <f t="shared" si="7"/>
+        <v>0.93500000000000005</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>8</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25">
+        <v>11062024</v>
+      </c>
+      <c r="F25" s="5">
+        <v>0.55277777777777781</v>
+      </c>
+      <c r="G25" s="5">
+        <v>0.57152777777777775</v>
+      </c>
+      <c r="I25">
+        <v>79.260000000000005</v>
+      </c>
+      <c r="J25">
+        <v>0.04</v>
+      </c>
+      <c r="K25">
+        <v>27</v>
+      </c>
+      <c r="R25">
+        <v>1.127</v>
+      </c>
+      <c r="S25">
+        <f>4994664+3526503+116244+2064552</f>
+        <v>10701963</v>
+      </c>
+      <c r="U25" s="4">
+        <f t="shared" si="4"/>
+        <v>47.947767007500005</v>
+      </c>
+      <c r="V25" s="4">
+        <f t="shared" si="5"/>
+        <v>0.81487174741789281</v>
+      </c>
+      <c r="W25" s="4">
+        <f t="shared" si="6"/>
+        <v>0.77911303860543846</v>
+      </c>
+      <c r="X25" s="4">
+        <f t="shared" si="7"/>
+        <v>1.127</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>8</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>11062024</v>
+      </c>
+      <c r="F26" s="5">
+        <v>0.55069444444444449</v>
+      </c>
+      <c r="G26" s="5">
+        <v>0.56527777777777777</v>
+      </c>
+      <c r="I26">
+        <v>185.96</v>
+      </c>
+      <c r="J26">
+        <v>0.04</v>
+      </c>
+      <c r="K26">
+        <v>26</v>
+      </c>
+      <c r="R26">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="S26">
+        <f>3250811+599022+1320192</f>
+        <v>5170025</v>
+      </c>
+      <c r="U26" s="4">
+        <f t="shared" si="4"/>
+        <v>23.163148118055556</v>
+      </c>
+      <c r="V26" s="4">
+        <f t="shared" si="5"/>
+        <v>34.046945257322065</v>
+      </c>
+      <c r="W26" s="4">
+        <f t="shared" si="6"/>
+        <v>33.287785826572019</v>
+      </c>
+      <c r="X26" s="4">
+        <f t="shared" si="7"/>
+        <v>0.13100000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
3rd species done with great graph
</commit_message>
<xml_diff>
--- a/data/Kleaf_Karli_Marion_CESE.xlsx
+++ b/data/Kleaf_Karli_Marion_CESE.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marion.boisseaux\Dropbox\Mon PC (Jaboty20)\Post_doc_CalState_LA\ScoffoniLab_Kleaf\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0468CD7-2961-4D84-91EE-825748F344BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0859F97D-3F3F-44B1-8B38-B85A1BE3536D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{63D1BA6E-C94C-4260-825C-85D06C6809A1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{63D1BA6E-C94C-4260-825C-85D06C6809A1}"/>
   </bookViews>
   <sheets>
     <sheet name="CESE" sheetId="1" r:id="rId1"/>
     <sheet name="PADI" sheetId="2" r:id="rId2"/>
+    <sheet name="AVSA" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CESE!$A$1:$AE$23</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="40">
   <si>
     <t>Specie</t>
   </si>
@@ -158,6 +159,9 @@
   <si>
     <t>could not do the potential, the leaf broke while doing it</t>
   </si>
+  <si>
+    <t>AVSA</t>
+  </si>
 </sst>
 </file>
 
@@ -233,7 +237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -255,6 +259,7 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2760,8 +2765,8 @@
   <dimension ref="A1:AE30"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD3"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3:F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4675,8 +4680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33064BB3-47FF-4DAF-9632-D6C75923AEEE}">
   <dimension ref="A1:AE26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="S4" sqref="S4"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6161,4 +6166,1118 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2FD146E-6B5C-415F-9192-209A980B6A9A}">
+  <dimension ref="A1:AE18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S19" sqref="S19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="17" width="0" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="0" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="V1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="W1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="X1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="8">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8">
+        <v>1</v>
+      </c>
+      <c r="D2" s="8">
+        <v>2</v>
+      </c>
+      <c r="E2" s="8">
+        <v>10222024</v>
+      </c>
+      <c r="F2" s="11">
+        <v>0.50208333333333333</v>
+      </c>
+      <c r="G2" s="11">
+        <v>0.52152777777777781</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="8">
+        <v>25.26</v>
+      </c>
+      <c r="J2" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="K2" s="12" t="e">
+        <f>AVERAGE(#REF!,#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M2" s="12"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="8">
+        <v>0.155</v>
+      </c>
+      <c r="S2" s="8">
+        <f>917270+813318+608426+406146</f>
+        <v>2745160</v>
+      </c>
+      <c r="U2" s="13">
+        <f>S2/(1200^2)*2.54^2</f>
+        <v>12.299079344444445</v>
+      </c>
+      <c r="V2" s="13">
+        <f>I2*0.000001/18*1000/R2/(U2/10000)</f>
+        <v>7.3613342814556653</v>
+      </c>
+      <c r="W2" s="13" t="e">
+        <f>V2/(0.88862*(1/POWER(10,(1.3272*(20-K2)-0.001053*(K2-20)^2)/(K2+105))))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="X2" s="13">
+        <f>MAX(Q2:R2)</f>
+        <v>0.155</v>
+      </c>
+      <c r="Z2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB2" s="14"/>
+      <c r="AC2" s="14"/>
+      <c r="AD2" s="13"/>
+      <c r="AE2" s="13"/>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>11072024</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0.37708333333333333</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0.39513888888888887</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3">
+        <v>44.13</v>
+      </c>
+      <c r="J3">
+        <v>0.06</v>
+      </c>
+      <c r="K3">
+        <v>26</v>
+      </c>
+      <c r="R3">
+        <v>1.468</v>
+      </c>
+      <c r="S3">
+        <f>5281756+1344062+349298</f>
+        <v>6975116</v>
+      </c>
+      <c r="U3" s="15">
+        <f t="shared" ref="U3:U8" si="0">S3/(1200^2)*2.54^2</f>
+        <v>31.250457212222223</v>
+      </c>
+      <c r="V3" s="15">
+        <f t="shared" ref="V3:V8" si="1">I3*0.000001/18*1000/R3/(U3/10000)</f>
+        <v>0.53441543266890212</v>
+      </c>
+      <c r="W3" s="15">
+        <f t="shared" ref="W3:W8" si="2">V3/(0.88862*(1/POWER(10,(1.3272*(20-K3)-0.001053*(K3-20)^2)/(K3+105))))</f>
+        <v>0.52249934114930507</v>
+      </c>
+      <c r="X3" s="15">
+        <f t="shared" ref="X3:X10" si="3">MAX(Q3:R3)</f>
+        <v>1.468</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>11072024</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0.38680555555555557</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0.40694444444444444</v>
+      </c>
+      <c r="H4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4">
+        <v>171.56</v>
+      </c>
+      <c r="J4">
+        <v>0.03</v>
+      </c>
+      <c r="K4">
+        <v>26</v>
+      </c>
+      <c r="R4">
+        <v>0.185</v>
+      </c>
+      <c r="S4">
+        <f>5045502+685140</f>
+        <v>5730642</v>
+      </c>
+      <c r="U4" s="15">
+        <f t="shared" si="0"/>
+        <v>25.674868005</v>
+      </c>
+      <c r="V4" s="15">
+        <f t="shared" si="1"/>
+        <v>20.066128289145034</v>
+      </c>
+      <c r="W4" s="15">
+        <f t="shared" si="2"/>
+        <v>19.618705167504814</v>
+      </c>
+      <c r="X4" s="15">
+        <f t="shared" si="3"/>
+        <v>0.185</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>11072024</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0.40347222222222223</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0.42222222222222222</v>
+      </c>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5">
+        <v>117.17</v>
+      </c>
+      <c r="J5">
+        <v>0.03</v>
+      </c>
+      <c r="K5">
+        <v>26</v>
+      </c>
+      <c r="R5">
+        <v>0.49099999999999999</v>
+      </c>
+      <c r="S5">
+        <f>8063160+963144+1127600</f>
+        <v>10153904</v>
+      </c>
+      <c r="U5" s="15">
+        <f t="shared" si="0"/>
+        <v>45.492310448888887</v>
+      </c>
+      <c r="V5" s="15">
+        <f t="shared" si="1"/>
+        <v>2.9142341191190404</v>
+      </c>
+      <c r="W5" s="15">
+        <f t="shared" si="2"/>
+        <v>2.8492541833796667</v>
+      </c>
+      <c r="X5" s="15">
+        <f t="shared" si="3"/>
+        <v>0.49099999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>11072024</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0.41111111111111109</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0.43333333333333335</v>
+      </c>
+      <c r="H6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6">
+        <v>110.97</v>
+      </c>
+      <c r="J6">
+        <v>0.05</v>
+      </c>
+      <c r="K6">
+        <v>25</v>
+      </c>
+      <c r="R6">
+        <v>0.246</v>
+      </c>
+      <c r="S6">
+        <f>6778726+1491326+1245354</f>
+        <v>9515406</v>
+      </c>
+      <c r="U6" s="15">
+        <f t="shared" si="0"/>
+        <v>42.631662048333332</v>
+      </c>
+      <c r="V6" s="15">
+        <f t="shared" si="1"/>
+        <v>5.8784889928390314</v>
+      </c>
+      <c r="W6" s="15">
+        <f t="shared" si="2"/>
+        <v>5.8789663163456787</v>
+      </c>
+      <c r="X6" s="15">
+        <f t="shared" si="3"/>
+        <v>0.246</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>11072024</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0.44374999999999998</v>
+      </c>
+      <c r="G7" s="5">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="H7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7">
+        <v>23.6</v>
+      </c>
+      <c r="J7">
+        <v>0.05</v>
+      </c>
+      <c r="K7">
+        <v>26</v>
+      </c>
+      <c r="R7">
+        <v>1.32</v>
+      </c>
+      <c r="S7">
+        <f>3760147+962550</f>
+        <v>4722697</v>
+      </c>
+      <c r="U7" s="15">
+        <f t="shared" si="0"/>
+        <v>21.158994420277779</v>
+      </c>
+      <c r="V7" s="15">
+        <f t="shared" si="1"/>
+        <v>0.46942967777055328</v>
+      </c>
+      <c r="W7" s="15">
+        <f t="shared" si="2"/>
+        <v>0.45896260167135966</v>
+      </c>
+      <c r="X7" s="15">
+        <f t="shared" si="3"/>
+        <v>1.32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>11072024</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0.47361111111111109</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0.48749999999999999</v>
+      </c>
+      <c r="H8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8">
+        <v>44.57</v>
+      </c>
+      <c r="J8">
+        <v>0.04</v>
+      </c>
+      <c r="K8">
+        <v>25</v>
+      </c>
+      <c r="R8">
+        <v>0.86</v>
+      </c>
+      <c r="S8">
+        <f>3183813+662040+666150</f>
+        <v>4512003</v>
+      </c>
+      <c r="U8" s="15">
+        <f t="shared" si="0"/>
+        <v>20.215026774166667</v>
+      </c>
+      <c r="V8" s="15">
+        <f t="shared" si="1"/>
+        <v>1.4242864966608282</v>
+      </c>
+      <c r="W8" s="15">
+        <f t="shared" si="2"/>
+        <v>1.42440214635004</v>
+      </c>
+      <c r="X8" s="15">
+        <f t="shared" si="3"/>
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>11082024</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0.38124999999999998</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="H9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9">
+        <v>58.06</v>
+      </c>
+      <c r="J9">
+        <v>0.06</v>
+      </c>
+      <c r="K9">
+        <v>26</v>
+      </c>
+      <c r="R9">
+        <v>1.617</v>
+      </c>
+      <c r="S9">
+        <f>6463264+2334373+298439</f>
+        <v>9096076</v>
+      </c>
+      <c r="U9" s="15">
+        <f t="shared" ref="U9:U13" si="4">S9/(1200^2)*2.54^2</f>
+        <v>40.752947167777776</v>
+      </c>
+      <c r="V9" s="15">
+        <f t="shared" ref="V9:V13" si="5">I9*0.000001/18*1000/R9/(U9/10000)</f>
+        <v>0.48948060145221556</v>
+      </c>
+      <c r="W9" s="15">
+        <f t="shared" ref="W9:W13" si="6">V9/(0.88862*(1/POWER(10,(1.3272*(20-K9)-0.001053*(K9-20)^2)/(K9+105))))</f>
+        <v>0.47856644125507602</v>
+      </c>
+      <c r="X9" s="15">
+        <f t="shared" ref="X9:X16" si="7">MAX(Q9:R9)</f>
+        <v>1.617</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>11082024</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0.40069444444444446</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0.41388888888888886</v>
+      </c>
+      <c r="H10" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10">
+        <v>51.6</v>
+      </c>
+      <c r="J10">
+        <v>0.03</v>
+      </c>
+      <c r="K10">
+        <v>25</v>
+      </c>
+      <c r="R10">
+        <v>0.91</v>
+      </c>
+      <c r="S10">
+        <f>5584263+814566+317757</f>
+        <v>6716586</v>
+      </c>
+      <c r="U10" s="15">
+        <f t="shared" si="4"/>
+        <v>30.09217099833333</v>
+      </c>
+      <c r="V10" s="15">
+        <f t="shared" si="5"/>
+        <v>1.0468447591759413</v>
+      </c>
+      <c r="W10" s="15">
+        <f t="shared" si="6"/>
+        <v>1.046929761225273</v>
+      </c>
+      <c r="X10" s="15">
+        <f t="shared" si="7"/>
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>11082024</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="G11" s="5">
+        <v>0.40486111111111112</v>
+      </c>
+      <c r="H11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11">
+        <v>71.3</v>
+      </c>
+      <c r="J11">
+        <v>0.03</v>
+      </c>
+      <c r="K11">
+        <v>25</v>
+      </c>
+      <c r="R11">
+        <v>0.51</v>
+      </c>
+      <c r="S11">
+        <f>5946627+808257+468075+163144</f>
+        <v>7386103</v>
+      </c>
+      <c r="U11" s="15">
+        <f t="shared" si="4"/>
+        <v>33.091793135277776</v>
+      </c>
+      <c r="V11" s="15">
+        <f t="shared" si="5"/>
+        <v>2.3470727318521951</v>
+      </c>
+      <c r="W11" s="15">
+        <f t="shared" si="6"/>
+        <v>2.3472633102453995</v>
+      </c>
+      <c r="X11" s="15">
+        <f t="shared" si="7"/>
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>11082024</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0.40972222222222221</v>
+      </c>
+      <c r="G12" s="5">
+        <v>0.4236111111111111</v>
+      </c>
+      <c r="H12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12">
+        <v>138.83000000000001</v>
+      </c>
+      <c r="J12">
+        <v>0.04</v>
+      </c>
+      <c r="K12">
+        <v>25</v>
+      </c>
+      <c r="R12">
+        <v>1.268</v>
+      </c>
+      <c r="S12">
+        <f>6214254+1622337+192996</f>
+        <v>8029587</v>
+      </c>
+      <c r="U12" s="15">
+        <f t="shared" ref="U12:U17" si="8">S12/(1200^2)*2.54^2</f>
+        <v>35.974780200833337</v>
+      </c>
+      <c r="V12" s="15">
+        <f t="shared" ref="V12:V17" si="9">I12*0.000001/18*1000/R12/(U12/10000)</f>
+        <v>1.6908045811266819</v>
+      </c>
+      <c r="W12" s="15">
+        <f t="shared" ref="W12:W17" si="10">V12/(0.88862*(1/POWER(10,(1.3272*(20-K12)-0.001053*(K12-20)^2)/(K12+105))))</f>
+        <v>1.6909418716400608</v>
+      </c>
+      <c r="X12" s="15">
+        <f t="shared" si="7"/>
+        <v>1.268</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>11082024</v>
+      </c>
+      <c r="F13" s="5">
+        <v>0.42986111111111114</v>
+      </c>
+      <c r="G13" s="5">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="H13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13">
+        <v>191.83</v>
+      </c>
+      <c r="J13">
+        <v>0.02</v>
+      </c>
+      <c r="K13">
+        <v>25</v>
+      </c>
+      <c r="R13">
+        <v>1.026</v>
+      </c>
+      <c r="S13">
+        <f>5773559+603204+274922</f>
+        <v>6651685</v>
+      </c>
+      <c r="U13" s="15">
+        <f t="shared" si="8"/>
+        <v>29.801396490277778</v>
+      </c>
+      <c r="V13" s="15">
+        <f t="shared" si="9"/>
+        <v>3.4854595372396737</v>
+      </c>
+      <c r="W13" s="15">
+        <f t="shared" si="10"/>
+        <v>3.4857425507437596</v>
+      </c>
+      <c r="X13" s="15">
+        <f t="shared" si="7"/>
+        <v>1.026</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>11082024</v>
+      </c>
+      <c r="F14" s="5">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="G14" s="5">
+        <v>0.43888888888888888</v>
+      </c>
+      <c r="H14" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14">
+        <v>121.13</v>
+      </c>
+      <c r="J14">
+        <v>0.04</v>
+      </c>
+      <c r="K14">
+        <v>26</v>
+      </c>
+      <c r="R14">
+        <v>0.67100000000000004</v>
+      </c>
+      <c r="S14">
+        <f>5654817+473235+62206</f>
+        <v>6190258</v>
+      </c>
+      <c r="U14" s="15">
+        <f t="shared" si="8"/>
+        <v>27.734075356111113</v>
+      </c>
+      <c r="V14" s="15">
+        <f t="shared" si="9"/>
+        <v>3.6161213881814085</v>
+      </c>
+      <c r="W14" s="15">
+        <f t="shared" si="10"/>
+        <v>3.5354911691169102</v>
+      </c>
+      <c r="X14" s="15">
+        <f t="shared" si="7"/>
+        <v>0.67100000000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>11082024</v>
+      </c>
+      <c r="F15" s="5">
+        <v>0.4548611111111111</v>
+      </c>
+      <c r="G15" s="5">
+        <v>0.46805555555555556</v>
+      </c>
+      <c r="H15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15">
+        <v>59.97</v>
+      </c>
+      <c r="J15">
+        <v>0.05</v>
+      </c>
+      <c r="K15">
+        <v>26</v>
+      </c>
+      <c r="R15">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="S15">
+        <f>4607082+209598</f>
+        <v>4816680</v>
+      </c>
+      <c r="U15" s="15">
+        <f t="shared" si="8"/>
+        <v>21.580064366666669</v>
+      </c>
+      <c r="V15" s="15">
+        <f t="shared" si="9"/>
+        <v>1.3908677242583791</v>
+      </c>
+      <c r="W15" s="15">
+        <f t="shared" si="10"/>
+        <v>1.3598549464066121</v>
+      </c>
+      <c r="X15" s="15">
+        <f t="shared" si="7"/>
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>11082024</v>
+      </c>
+      <c r="F16" s="5">
+        <v>0.4548611111111111</v>
+      </c>
+      <c r="G16" s="5">
+        <v>0.47291666666666665</v>
+      </c>
+      <c r="H16" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16">
+        <v>101.23</v>
+      </c>
+      <c r="J16">
+        <v>0.05</v>
+      </c>
+      <c r="K16">
+        <v>25</v>
+      </c>
+      <c r="R16">
+        <v>0.128</v>
+      </c>
+      <c r="S16">
+        <f>4592508+1761562</f>
+        <v>6354070</v>
+      </c>
+      <c r="U16" s="15">
+        <f t="shared" si="8"/>
+        <v>28.467998619444444</v>
+      </c>
+      <c r="V16" s="15">
+        <f t="shared" si="9"/>
+        <v>15.433691890948205</v>
+      </c>
+      <c r="W16" s="15">
+        <f t="shared" si="10"/>
+        <v>15.434945081001445</v>
+      </c>
+      <c r="X16" s="15">
+        <f t="shared" si="7"/>
+        <v>0.128</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>6</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>11082024</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0.4777777777777778</v>
+      </c>
+      <c r="G17" s="5">
+        <v>0.49166666666666664</v>
+      </c>
+      <c r="H17" t="s">
+        <v>28</v>
+      </c>
+      <c r="I17">
+        <v>67</v>
+      </c>
+      <c r="J17">
+        <v>0.04</v>
+      </c>
+      <c r="K17">
+        <v>27</v>
+      </c>
+      <c r="R17">
+        <v>1.57</v>
+      </c>
+      <c r="S17">
+        <f>4791126+404936</f>
+        <v>5196062</v>
+      </c>
+      <c r="U17" s="15">
+        <f t="shared" ref="U17:U18" si="11">S17/(1200^2)*2.54^2</f>
+        <v>23.279801110555557</v>
+      </c>
+      <c r="V17" s="15">
+        <f t="shared" ref="V17:V18" si="12">I17*0.000001/18*1000/R17/(U17/10000)</f>
+        <v>1.0184116988372323</v>
+      </c>
+      <c r="W17" s="15">
+        <f t="shared" ref="W17:W18" si="13">V17/(0.88862*(1/POWER(10,(1.3272*(20-K17)-0.001053*(K17-20)^2)/(K17+105))))</f>
+        <v>0.97372112328922322</v>
+      </c>
+      <c r="X17" s="15">
+        <f t="shared" ref="X17:X18" si="14">MAX(Q17:R17)</f>
+        <v>1.57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>6</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>11082024</v>
+      </c>
+      <c r="F18" s="5">
+        <v>0.48680555555555555</v>
+      </c>
+      <c r="G18" s="5">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="H18" t="s">
+        <v>28</v>
+      </c>
+      <c r="I18">
+        <v>26.43</v>
+      </c>
+      <c r="J18">
+        <v>0.05</v>
+      </c>
+      <c r="K18">
+        <v>25</v>
+      </c>
+      <c r="R18">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="S18">
+        <f>4186731+1475286</f>
+        <v>5662017</v>
+      </c>
+      <c r="U18" s="15">
+        <f t="shared" si="11"/>
+        <v>25.367408942499999</v>
+      </c>
+      <c r="V18" s="15">
+        <f t="shared" si="12"/>
+        <v>4.1943962989973738</v>
+      </c>
+      <c r="W18" s="15">
+        <f t="shared" si="13"/>
+        <v>4.1947368769847007</v>
+      </c>
+      <c r="X18" s="15">
+        <f t="shared" si="14"/>
+        <v>0.13800000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update for 13 dec 2024
</commit_message>
<xml_diff>
--- a/data/Kleaf_Karli_Marion_CESE.xlsx
+++ b/data/Kleaf_Karli_Marion_CESE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marion.boisseaux\Dropbox\Mon PC (Jaboty20)\Post_doc_CalState_LA\ScoffoniLab_Kleaf\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A534756-C8CC-40D0-A5A7-4CB0C965DCC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8711D48D-471C-4355-803A-01C9933B2A0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{63D1BA6E-C94C-4260-825C-85D06C6809A1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{63D1BA6E-C94C-4260-825C-85D06C6809A1}"/>
   </bookViews>
   <sheets>
     <sheet name="CESE" sheetId="1" r:id="rId1"/>
@@ -19,11 +19,12 @@
     <sheet name="STDE" sheetId="4" r:id="rId4"/>
     <sheet name="DASP" sheetId="5" r:id="rId5"/>
     <sheet name="CHLA" sheetId="6" r:id="rId6"/>
+    <sheet name="ZEMA" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CESE!$A$1:$AE$23</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="70">
   <si>
     <t>Specie</t>
   </si>
@@ -221,6 +222,39 @@
   </si>
   <si>
     <t>very low flow but was stable</t>
+  </si>
+  <si>
+    <t>ZEMA</t>
+  </si>
+  <si>
+    <t>no PsiLeaf, leaf broke</t>
+  </si>
+  <si>
+    <t>the leaf was smooched, not ideal, need to find better fitting</t>
+  </si>
+  <si>
+    <t>first bubbles at 0.024</t>
+  </si>
+  <si>
+    <t>long wait because was interrupted by tax form department</t>
+  </si>
+  <si>
+    <t>shorter leaf for the pressure bomb, measured at leaf tip around 9 cm</t>
+  </si>
+  <si>
+    <t>one hour to stabilise, very weird</t>
+  </si>
+  <si>
+    <t xml:space="preserve">but there was a leak so start'again' at 09:09 but then was really stable </t>
+  </si>
+  <si>
+    <t>running cv 0.02, stable</t>
+  </si>
+  <si>
+    <t>running cv 0.01 very stable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">running cv 0.01 </t>
   </si>
 </sst>
 </file>
@@ -4739,7 +4773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33064BB3-47FF-4DAF-9632-D6C75923AEEE}">
   <dimension ref="A1:AE26"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3:E26"/>
     </sheetView>
   </sheetViews>
@@ -7343,10 +7377,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F80EEFC-0235-4E88-9007-0CE0804F1C9F}">
-  <dimension ref="A1:AE23"/>
+  <dimension ref="A1:AE29"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="D5" workbookViewId="0">
+      <selection activeCell="AA27" sqref="AA27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8580,7 +8614,7 @@
         <v>3.1938569589454042</v>
       </c>
       <c r="X20" s="4">
-        <f t="shared" ref="X20:X23" si="14">MAX(Q20:R20)</f>
+        <f t="shared" ref="X20:X29" si="14">MAX(Q20:R20)</f>
         <v>0.67500000000000004</v>
       </c>
     </row>
@@ -8765,6 +8799,345 @@
       </c>
       <c r="Z23" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>7</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>12122024</v>
+      </c>
+      <c r="F24" s="5">
+        <v>0.51736111111111116</v>
+      </c>
+      <c r="G24" s="5">
+        <v>0.53611111111111109</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>11.7</v>
+      </c>
+      <c r="J24">
+        <v>0.1</v>
+      </c>
+      <c r="K24">
+        <v>23</v>
+      </c>
+      <c r="R24">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="S24">
+        <v>1849785</v>
+      </c>
+      <c r="U24" s="4">
+        <f t="shared" ref="U24:U29" si="15">S24/(1200^2)*2.54^2</f>
+        <v>8.2875506291666667</v>
+      </c>
+      <c r="V24" s="4">
+        <f t="shared" ref="V24:V29" si="16">I24*0.000001/18*1000/R24/(U24/10000)</f>
+        <v>10.18583031257724</v>
+      </c>
+      <c r="W24" s="4">
+        <f t="shared" ref="W24:W29" si="17">V24/(0.88862*(1/POWER(10,(1.3272*(20-K24)-0.001053*(K24-20)^2)/(K24+105))))</f>
+        <v>10.668419001876826</v>
+      </c>
+      <c r="X24" s="4">
+        <f t="shared" si="14"/>
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>8</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>12122024</v>
+      </c>
+      <c r="F25" s="5">
+        <v>0.54027777777777775</v>
+      </c>
+      <c r="G25" s="5">
+        <v>0.55347222222222225</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>34.270000000000003</v>
+      </c>
+      <c r="J25">
+        <v>0.05</v>
+      </c>
+      <c r="K25">
+        <v>23</v>
+      </c>
+      <c r="R25">
+        <v>0.104</v>
+      </c>
+      <c r="S25">
+        <v>3017289</v>
+      </c>
+      <c r="U25" s="4">
+        <f t="shared" si="15"/>
+        <v>13.518292855833332</v>
+      </c>
+      <c r="V25" s="4">
+        <f t="shared" si="16"/>
+        <v>13.542112252527783</v>
+      </c>
+      <c r="W25" s="4">
+        <f t="shared" si="17"/>
+        <v>14.183716324237642</v>
+      </c>
+      <c r="X25" s="4">
+        <f t="shared" si="14"/>
+        <v>0.104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>9</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+      <c r="E26">
+        <v>12122024</v>
+      </c>
+      <c r="F26" s="5">
+        <v>0.54861111111111116</v>
+      </c>
+      <c r="G26" s="5">
+        <v>0.56111111111111112</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>32.6</v>
+      </c>
+      <c r="J26">
+        <v>0.05</v>
+      </c>
+      <c r="K26">
+        <v>23</v>
+      </c>
+      <c r="R26">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="U26" s="4">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="V26" s="4" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W26" s="4" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X26" s="4">
+        <f t="shared" si="14"/>
+        <v>0.14899999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>10</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>12122024</v>
+      </c>
+      <c r="F27" s="5">
+        <v>0.55902777777777779</v>
+      </c>
+      <c r="G27" s="5">
+        <v>0.5756944444444444</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>65.2</v>
+      </c>
+      <c r="J27">
+        <v>0.04</v>
+      </c>
+      <c r="K27">
+        <v>24</v>
+      </c>
+      <c r="R27">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="U27" s="4">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="V27" s="4" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W27" s="4" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X27" s="4">
+        <f t="shared" si="14"/>
+        <v>0.32300000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>11</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28">
+        <v>12122024</v>
+      </c>
+      <c r="F28" s="5">
+        <v>0.56666666666666665</v>
+      </c>
+      <c r="G28" s="5">
+        <v>0.57916666666666672</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>23.17</v>
+      </c>
+      <c r="J28">
+        <v>0.06</v>
+      </c>
+      <c r="K28">
+        <v>23</v>
+      </c>
+      <c r="R28">
+        <v>0.104</v>
+      </c>
+      <c r="U28" s="4">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="V28" s="4" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W28" s="4" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X28" s="4">
+        <f t="shared" si="14"/>
+        <v>0.104</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>12</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>12122024</v>
+      </c>
+      <c r="F29" s="5">
+        <v>0.58194444444444449</v>
+      </c>
+      <c r="G29" s="5">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>13.47</v>
+      </c>
+      <c r="J29">
+        <v>0.09</v>
+      </c>
+      <c r="K29">
+        <v>24</v>
+      </c>
+      <c r="R29">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="U29" s="4">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="V29" s="4" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W29" s="4" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X29" s="4">
+        <f t="shared" si="14"/>
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -10230,9 +10603,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E21FF7F-5593-4259-A4BA-F4FE44134BEE}">
   <dimension ref="A1:AG1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U34" sqref="U34"/>
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12626,4 +12999,1901 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58711BA0-843B-41FF-A312-D39246D429D2}">
+  <dimension ref="A1:AE32"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="W34" sqref="W34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.6640625" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="19.21875" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="6.5546875" hidden="1" customWidth="1"/>
+    <col min="15" max="16" width="17.21875" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="17.44140625" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="0" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="V1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="W1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="X1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="8">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8">
+        <v>1</v>
+      </c>
+      <c r="D2" s="8">
+        <v>2</v>
+      </c>
+      <c r="E2" s="8">
+        <v>10222024</v>
+      </c>
+      <c r="F2" s="11">
+        <v>0.50208333333333333</v>
+      </c>
+      <c r="G2" s="11">
+        <v>0.52152777777777781</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="8">
+        <v>25.26</v>
+      </c>
+      <c r="J2" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="K2" s="12" t="e">
+        <f>AVERAGE(#REF!,#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M2" s="12"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="8">
+        <v>0.155</v>
+      </c>
+      <c r="S2" s="8">
+        <f>917270+813318+608426+406146</f>
+        <v>2745160</v>
+      </c>
+      <c r="U2" s="13">
+        <f>S2/(1200^2)*2.54^2</f>
+        <v>12.299079344444445</v>
+      </c>
+      <c r="V2" s="13">
+        <f>I2*0.000001/18*1000/R2/(U2/10000)</f>
+        <v>7.3613342814556653</v>
+      </c>
+      <c r="W2" s="13" t="e">
+        <f>V2/(0.88862*(1/POWER(10,(1.3272*(20-K2)-0.001053*(K2-20)^2)/(K2+105))))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="X2" s="13">
+        <f>MAX(Q2:R2)</f>
+        <v>0.155</v>
+      </c>
+      <c r="Z2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB2" s="14"/>
+      <c r="AC2" s="14"/>
+      <c r="AD2" s="13"/>
+      <c r="AE2" s="13"/>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>12052024</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0.62013888888888891</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3">
+        <v>43.73</v>
+      </c>
+      <c r="J3">
+        <v>0.04</v>
+      </c>
+      <c r="K3">
+        <v>26</v>
+      </c>
+      <c r="U3" s="4">
+        <f t="shared" ref="U3:U18" si="0">S3/(1200^2)*2.54^2</f>
+        <v>0</v>
+      </c>
+      <c r="V3" s="4" t="e">
+        <f t="shared" ref="V3:V18" si="1">I3*0.000001/18*1000/R3/(U3/10000)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W3" s="4" t="e">
+        <f t="shared" ref="W3:W18" si="2">V3/(0.88862*(1/POWER(10,(1.3272*(20-K3)-0.001053*(K3-20)^2)/(K3+105))))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X3" s="4">
+        <f t="shared" ref="X3:X32" si="3">MAX(Q3:R3)</f>
+        <v>0</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>12052024</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="H4" t="s">
+        <v>28</v>
+      </c>
+      <c r="U4" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V4" s="4" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W4" s="4" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X4" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>12062024</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0.54374999999999996</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0.55833333333333335</v>
+      </c>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5">
+        <v>62</v>
+      </c>
+      <c r="J5">
+        <v>0.05</v>
+      </c>
+      <c r="K5">
+        <v>26</v>
+      </c>
+      <c r="R5">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="S5">
+        <v>13378965</v>
+      </c>
+      <c r="U5" s="4">
+        <f t="shared" si="0"/>
+        <v>59.941479579166668</v>
+      </c>
+      <c r="V5" s="4">
+        <f t="shared" si="1"/>
+        <v>6.6817969572582454</v>
+      </c>
+      <c r="W5" s="4">
+        <f t="shared" si="2"/>
+        <v>6.5328100470928279</v>
+      </c>
+      <c r="X5" s="4">
+        <f t="shared" si="3"/>
+        <v>8.5999999999999993E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>12062024</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0.55486111111111114</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0.57847222222222228</v>
+      </c>
+      <c r="H6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6">
+        <v>121.93</v>
+      </c>
+      <c r="J6">
+        <v>0.03</v>
+      </c>
+      <c r="K6">
+        <v>26</v>
+      </c>
+      <c r="R6">
+        <v>0.27800000000000002</v>
+      </c>
+      <c r="S6">
+        <v>15255156</v>
+      </c>
+      <c r="U6" s="4">
+        <f t="shared" si="0"/>
+        <v>68.347336423333331</v>
+      </c>
+      <c r="V6" s="4">
+        <f t="shared" si="1"/>
+        <v>3.5650996907387573</v>
+      </c>
+      <c r="W6" s="4">
+        <f t="shared" si="2"/>
+        <v>3.4856071244796349</v>
+      </c>
+      <c r="X6" s="4">
+        <f t="shared" si="3"/>
+        <v>0.27800000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>12062024</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0.57361111111111107</v>
+      </c>
+      <c r="G7" s="5">
+        <v>0.58958333333333335</v>
+      </c>
+      <c r="H7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7">
+        <v>123.17</v>
+      </c>
+      <c r="J7">
+        <v>0.05</v>
+      </c>
+      <c r="K7">
+        <v>25</v>
+      </c>
+      <c r="R7">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="S7">
+        <v>13119866</v>
+      </c>
+      <c r="U7" s="4">
+        <f t="shared" si="0"/>
+        <v>58.780644087222228</v>
+      </c>
+      <c r="V7" s="4">
+        <f>I7*0.000001/18*1000/K7/(U7/10000)</f>
+        <v>4.65648370073935E-2</v>
+      </c>
+      <c r="W7" s="4">
+        <f>V7/(0.88862*(1/POWER(10,(1.3272*(20-R7)-0.001053*(R7-20)^2)/(R7+105))))</f>
+        <v>9.2709282164009865E-2</v>
+      </c>
+      <c r="X7" s="4">
+        <f>MAX(R7:R7)</f>
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>12062024</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0.58888888888888891</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0.60347222222222219</v>
+      </c>
+      <c r="H8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8">
+        <v>76.73</v>
+      </c>
+      <c r="J8">
+        <v>0.03</v>
+      </c>
+      <c r="K8">
+        <v>25</v>
+      </c>
+      <c r="R8">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="S8">
+        <v>14134963</v>
+      </c>
+      <c r="U8" s="4">
+        <f t="shared" si="0"/>
+        <v>63.328560618611107</v>
+      </c>
+      <c r="V8" s="4">
+        <f>I8*0.000001/18*1000/K8/(U8/10000)</f>
+        <v>2.6924836036933558E-2</v>
+      </c>
+      <c r="W8" s="4">
+        <f>V8/(0.88862*(1/POWER(10,(1.3272*(20-R8)-0.001053*(R8-20)^2)/(R8+105))))</f>
+        <v>5.267191150476299E-2</v>
+      </c>
+      <c r="X8" s="4">
+        <f>MAX(R8:R8)</f>
+        <v>0.59499999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>12062024</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0.59861111111111109</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0.62708333333333333</v>
+      </c>
+      <c r="H9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9">
+        <v>188.77</v>
+      </c>
+      <c r="J9">
+        <v>0.01</v>
+      </c>
+      <c r="K9">
+        <v>24</v>
+      </c>
+      <c r="R9">
+        <v>0.08</v>
+      </c>
+      <c r="S9">
+        <v>13385285</v>
+      </c>
+      <c r="U9" s="4">
+        <f t="shared" si="0"/>
+        <v>59.969794934722223</v>
+      </c>
+      <c r="V9" s="4">
+        <f t="shared" si="1"/>
+        <v>21.859384031656429</v>
+      </c>
+      <c r="W9" s="4">
+        <f t="shared" si="2"/>
+        <v>22.368545398229067</v>
+      </c>
+      <c r="X9" s="4">
+        <f t="shared" si="3"/>
+        <v>0.08</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>12102024</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0.37291666666666667</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0.40555555555555556</v>
+      </c>
+      <c r="H10" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="J10">
+        <v>0.06</v>
+      </c>
+      <c r="K10">
+        <v>26</v>
+      </c>
+      <c r="R10">
+        <v>0.87</v>
+      </c>
+      <c r="S10">
+        <v>13030974</v>
+      </c>
+      <c r="U10" s="4">
+        <f t="shared" si="0"/>
+        <v>58.382383234999999</v>
+      </c>
+      <c r="V10" s="4">
+        <f t="shared" si="1"/>
+        <v>0.44625858697601511</v>
+      </c>
+      <c r="W10" s="4">
+        <f t="shared" si="2"/>
+        <v>0.43630816668733524</v>
+      </c>
+      <c r="X10" s="4">
+        <f t="shared" si="3"/>
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>12102024</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0.41180555555555554</v>
+      </c>
+      <c r="G11" s="5">
+        <v>0.42777777777777776</v>
+      </c>
+      <c r="H11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11">
+        <v>79.2</v>
+      </c>
+      <c r="J11">
+        <v>0.02</v>
+      </c>
+      <c r="K11">
+        <v>26</v>
+      </c>
+      <c r="R11">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="S11">
+        <v>20417957</v>
+      </c>
+      <c r="U11" s="4">
+        <f t="shared" si="0"/>
+        <v>91.478119014722225</v>
+      </c>
+      <c r="V11" s="4">
+        <f t="shared" si="1"/>
+        <v>2.9328618233137371</v>
+      </c>
+      <c r="W11" s="4">
+        <f t="shared" si="2"/>
+        <v>2.8674665376154831</v>
+      </c>
+      <c r="X11" s="4">
+        <f t="shared" si="3"/>
+        <v>0.16400000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>12102024</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0.38333333333333336</v>
+      </c>
+      <c r="G12" s="5">
+        <v>0.40138888888888891</v>
+      </c>
+      <c r="H12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12">
+        <v>261.93</v>
+      </c>
+      <c r="J12">
+        <v>0.01</v>
+      </c>
+      <c r="K12">
+        <v>25</v>
+      </c>
+      <c r="R12">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="S12">
+        <v>16946131</v>
+      </c>
+      <c r="U12" s="4">
+        <f t="shared" si="0"/>
+        <v>75.923374138611123</v>
+      </c>
+      <c r="V12" s="4">
+        <f t="shared" si="1"/>
+        <v>21.061817486731385</v>
+      </c>
+      <c r="W12" s="4">
+        <f t="shared" si="2"/>
+        <v>21.063527671200792</v>
+      </c>
+      <c r="X12" s="4">
+        <f t="shared" si="3"/>
+        <v>9.0999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13">
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>12102024</v>
+      </c>
+      <c r="F13" s="5">
+        <v>0.43263888888888891</v>
+      </c>
+      <c r="G13" s="5">
+        <v>0.44583333333333336</v>
+      </c>
+      <c r="H13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13">
+        <v>112.9</v>
+      </c>
+      <c r="J13">
+        <v>0.05</v>
+      </c>
+      <c r="K13">
+        <v>25</v>
+      </c>
+      <c r="R13">
+        <v>4.7E-2</v>
+      </c>
+      <c r="S13">
+        <v>15465925</v>
+      </c>
+      <c r="U13" s="4">
+        <f t="shared" si="0"/>
+        <v>69.291640090277781</v>
+      </c>
+      <c r="V13" s="4">
+        <f t="shared" si="1"/>
+        <v>19.25939932568437</v>
+      </c>
+      <c r="W13" s="4">
+        <f t="shared" si="2"/>
+        <v>19.260963156803772</v>
+      </c>
+      <c r="X13" s="4">
+        <f t="shared" si="3"/>
+        <v>4.7E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>12102024</v>
+      </c>
+      <c r="F14" s="5">
+        <v>0.43541666666666667</v>
+      </c>
+      <c r="G14" s="5">
+        <v>0.44861111111111113</v>
+      </c>
+      <c r="H14" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14">
+        <v>232.6</v>
+      </c>
+      <c r="J14">
+        <v>0.02</v>
+      </c>
+      <c r="K14">
+        <v>26</v>
+      </c>
+      <c r="R14">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="S14">
+        <v>13527094</v>
+      </c>
+      <c r="U14" s="4">
+        <f t="shared" si="0"/>
+        <v>60.605138646111108</v>
+      </c>
+      <c r="V14" s="4">
+        <f t="shared" si="1"/>
+        <v>14.806938211129051</v>
+      </c>
+      <c r="W14" s="4">
+        <f t="shared" si="2"/>
+        <v>14.476781520167345</v>
+      </c>
+      <c r="X14" s="4">
+        <f t="shared" si="3"/>
+        <v>0.14399999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>12102024</v>
+      </c>
+      <c r="F15" s="5">
+        <v>0.41041666666666665</v>
+      </c>
+      <c r="G15" s="5">
+        <v>0.42638888888888887</v>
+      </c>
+      <c r="H15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15">
+        <v>79.2</v>
+      </c>
+      <c r="J15">
+        <v>0.05</v>
+      </c>
+      <c r="K15">
+        <v>26</v>
+      </c>
+      <c r="R15">
+        <v>0.155</v>
+      </c>
+      <c r="S15">
+        <v>8803209</v>
+      </c>
+      <c r="U15" s="4">
+        <f t="shared" si="0"/>
+        <v>39.440821655833332</v>
+      </c>
+      <c r="V15" s="4">
+        <f t="shared" si="1"/>
+        <v>7.1973898064050781</v>
+      </c>
+      <c r="W15" s="4">
+        <f t="shared" si="2"/>
+        <v>7.0369064999874027</v>
+      </c>
+      <c r="X15" s="4">
+        <f t="shared" si="3"/>
+        <v>0.155</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>12102024</v>
+      </c>
+      <c r="F16" s="5">
+        <v>0.63055555555555554</v>
+      </c>
+      <c r="G16" s="5">
+        <v>0.67083333333333328</v>
+      </c>
+      <c r="H16" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16">
+        <v>201.47</v>
+      </c>
+      <c r="J16">
+        <v>0.04</v>
+      </c>
+      <c r="K16">
+        <v>24</v>
+      </c>
+      <c r="R16">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="S16">
+        <v>21421647</v>
+      </c>
+      <c r="U16" s="4">
+        <f t="shared" si="0"/>
+        <v>95.974929017500003</v>
+      </c>
+      <c r="V16" s="4">
+        <f t="shared" si="1"/>
+        <v>2.0975160377667299</v>
+      </c>
+      <c r="W16" s="4">
+        <f t="shared" si="2"/>
+        <v>2.1463725897469095</v>
+      </c>
+      <c r="X16" s="4">
+        <f t="shared" si="3"/>
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>12102024</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="G17" s="5">
+        <v>0.48125000000000001</v>
+      </c>
+      <c r="H17" t="s">
+        <v>28</v>
+      </c>
+      <c r="I17">
+        <v>160.77000000000001</v>
+      </c>
+      <c r="J17">
+        <v>0.03</v>
+      </c>
+      <c r="K17">
+        <v>26</v>
+      </c>
+      <c r="R17">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="S17">
+        <v>12640218</v>
+      </c>
+      <c r="U17" s="4">
+        <f t="shared" si="0"/>
+        <v>56.631687811666666</v>
+      </c>
+      <c r="V17" s="4">
+        <f t="shared" si="1"/>
+        <v>18.554705931067421</v>
+      </c>
+      <c r="W17" s="4">
+        <f t="shared" si="2"/>
+        <v>18.140983645972423</v>
+      </c>
+      <c r="X17" s="4">
+        <f t="shared" si="3"/>
+        <v>8.5000000000000006E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>12102024</v>
+      </c>
+      <c r="F18" s="5">
+        <v>0.64444444444444449</v>
+      </c>
+      <c r="G18" s="5">
+        <v>0.66597222222222219</v>
+      </c>
+      <c r="H18" t="s">
+        <v>28</v>
+      </c>
+      <c r="I18">
+        <v>109.33</v>
+      </c>
+      <c r="J18">
+        <v>0.05</v>
+      </c>
+      <c r="K18">
+        <v>25</v>
+      </c>
+      <c r="R18">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="S18">
+        <v>14173680</v>
+      </c>
+      <c r="U18" s="4">
+        <f t="shared" si="0"/>
+        <v>63.502023533333329</v>
+      </c>
+      <c r="V18" s="4">
+        <f t="shared" si="1"/>
+        <v>2.2611996576623818</v>
+      </c>
+      <c r="W18" s="4">
+        <f t="shared" si="2"/>
+        <v>2.2613832633051141</v>
+      </c>
+      <c r="X18" s="4">
+        <f t="shared" si="3"/>
+        <v>0.42299999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>12112024</v>
+      </c>
+      <c r="F19" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="G19" s="5">
+        <v>0.39097222222222222</v>
+      </c>
+      <c r="H19" t="s">
+        <v>28</v>
+      </c>
+      <c r="I19">
+        <v>148.77000000000001</v>
+      </c>
+      <c r="J19">
+        <v>0.04</v>
+      </c>
+      <c r="K19">
+        <v>24</v>
+      </c>
+      <c r="R19">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="S19">
+        <v>20908017</v>
+      </c>
+      <c r="U19" s="4">
+        <f t="shared" ref="U19:U28" si="4">S19/(1200^2)*2.54^2</f>
+        <v>93.67372394249999</v>
+      </c>
+      <c r="V19" s="4">
+        <f t="shared" ref="V19:V28" si="5">I19*0.000001/18*1000/R19/(U19/10000)</f>
+        <v>1.5344658500287061</v>
+      </c>
+      <c r="W19" s="4">
+        <f t="shared" ref="W19:W28" si="6">V19/(0.88862*(1/POWER(10,(1.3272*(20-K19)-0.001053*(K19-20)^2)/(K19+105))))</f>
+        <v>1.5702075126495834</v>
+      </c>
+      <c r="X19" s="4">
+        <f t="shared" si="3"/>
+        <v>0.57499999999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20">
+        <v>6</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>12112024</v>
+      </c>
+      <c r="F20" s="5">
+        <v>0.38680555555555557</v>
+      </c>
+      <c r="G20" s="5">
+        <v>0.40138888888888891</v>
+      </c>
+      <c r="H20" t="s">
+        <v>28</v>
+      </c>
+      <c r="I20">
+        <v>258.5</v>
+      </c>
+      <c r="J20">
+        <v>0.01</v>
+      </c>
+      <c r="K20">
+        <v>25</v>
+      </c>
+      <c r="R20">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="S20">
+        <v>26332259</v>
+      </c>
+      <c r="U20" s="4">
+        <f t="shared" si="4"/>
+        <v>117.97583483638888</v>
+      </c>
+      <c r="V20" s="4">
+        <f t="shared" si="5"/>
+        <v>6.7253734987373246</v>
+      </c>
+      <c r="W20" s="4">
+        <f t="shared" si="6"/>
+        <v>6.7259195878540758</v>
+      </c>
+      <c r="X20" s="4">
+        <f t="shared" si="3"/>
+        <v>0.18099999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21">
+        <v>6</v>
+      </c>
+      <c r="C21">
+        <v>5</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <v>12112024</v>
+      </c>
+      <c r="F21" s="5">
+        <v>0.3972222222222222</v>
+      </c>
+      <c r="G21" s="5">
+        <v>0.41111111111111109</v>
+      </c>
+      <c r="H21" t="s">
+        <v>28</v>
+      </c>
+      <c r="I21">
+        <v>120.67</v>
+      </c>
+      <c r="J21">
+        <v>0.03</v>
+      </c>
+      <c r="K21">
+        <v>25</v>
+      </c>
+      <c r="R21">
+        <v>0.433</v>
+      </c>
+      <c r="S21">
+        <v>16172823</v>
+      </c>
+      <c r="U21" s="4">
+        <f t="shared" si="4"/>
+        <v>72.458739490833338</v>
+      </c>
+      <c r="V21" s="4">
+        <f t="shared" si="5"/>
+        <v>2.136722565832859</v>
+      </c>
+      <c r="W21" s="4">
+        <f t="shared" si="6"/>
+        <v>2.1368960641432411</v>
+      </c>
+      <c r="X21" s="4">
+        <f t="shared" si="3"/>
+        <v>0.433</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <v>5</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>12112024</v>
+      </c>
+      <c r="F22" s="5">
+        <v>0.40763888888888888</v>
+      </c>
+      <c r="G22" s="5">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="H22" t="s">
+        <v>28</v>
+      </c>
+      <c r="I22">
+        <v>203.57</v>
+      </c>
+      <c r="J22">
+        <v>0.03</v>
+      </c>
+      <c r="K22">
+        <v>25</v>
+      </c>
+      <c r="R22">
+        <v>0.66400000000000003</v>
+      </c>
+      <c r="S22">
+        <v>17956261</v>
+      </c>
+      <c r="U22" s="4">
+        <f t="shared" si="4"/>
+        <v>80.449037130277773</v>
+      </c>
+      <c r="V22" s="4">
+        <f t="shared" si="5"/>
+        <v>2.1171534747501242</v>
+      </c>
+      <c r="W22" s="4">
+        <f t="shared" si="6"/>
+        <v>2.1173253840829322</v>
+      </c>
+      <c r="X22" s="4">
+        <f t="shared" si="3"/>
+        <v>0.66400000000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="C23">
+        <v>6</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23">
+        <v>12112024</v>
+      </c>
+      <c r="F23" s="5">
+        <v>0.43402777777777779</v>
+      </c>
+      <c r="G23" s="5">
+        <v>0.44722222222222224</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>20.7</v>
+      </c>
+      <c r="J23">
+        <v>0.05</v>
+      </c>
+      <c r="K23">
+        <v>23</v>
+      </c>
+      <c r="R23">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="S23">
+        <v>8346696</v>
+      </c>
+      <c r="U23" s="4">
+        <f t="shared" si="4"/>
+        <v>37.395516606666668</v>
+      </c>
+      <c r="V23" s="4">
+        <f t="shared" si="5"/>
+        <v>2.3475076027251531</v>
+      </c>
+      <c r="W23" s="4">
+        <f t="shared" si="6"/>
+        <v>2.4587288367683997</v>
+      </c>
+      <c r="X23" s="4">
+        <f t="shared" si="3"/>
+        <v>0.13100000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24">
+        <v>7</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>12112024</v>
+      </c>
+      <c r="F24" s="5">
+        <v>0.44305555555555554</v>
+      </c>
+      <c r="G24" s="5">
+        <v>0.46180555555555558</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>23.4</v>
+      </c>
+      <c r="J24">
+        <v>0.05</v>
+      </c>
+      <c r="K24">
+        <v>24</v>
+      </c>
+      <c r="R24">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="S24">
+        <v>16308608</v>
+      </c>
+      <c r="U24" s="4">
+        <f t="shared" si="4"/>
+        <v>73.067094008888887</v>
+      </c>
+      <c r="V24" s="4">
+        <f t="shared" si="5"/>
+        <v>3.3569559894921359</v>
+      </c>
+      <c r="W24" s="4">
+        <f t="shared" si="6"/>
+        <v>3.4351481424209984</v>
+      </c>
+      <c r="X24" s="4">
+        <f t="shared" si="3"/>
+        <v>5.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25">
+        <v>7</v>
+      </c>
+      <c r="C25">
+        <v>5</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25">
+        <v>12112024</v>
+      </c>
+      <c r="F25" s="5">
+        <v>0.45416666666666666</v>
+      </c>
+      <c r="G25" s="5">
+        <v>0.46736111111111112</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>35.53</v>
+      </c>
+      <c r="J25">
+        <v>0.03</v>
+      </c>
+      <c r="K25">
+        <v>24</v>
+      </c>
+      <c r="R25">
+        <v>5.5E-2</v>
+      </c>
+      <c r="S25">
+        <v>22384129</v>
+      </c>
+      <c r="U25" s="4">
+        <f t="shared" si="4"/>
+        <v>100.2871157336111</v>
+      </c>
+      <c r="V25" s="4">
+        <f t="shared" si="5"/>
+        <v>3.5786141246916698</v>
+      </c>
+      <c r="W25" s="4">
+        <f t="shared" si="6"/>
+        <v>3.6619692666080854</v>
+      </c>
+      <c r="X25" s="4">
+        <f t="shared" si="3"/>
+        <v>5.5E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26">
+        <v>4</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+      <c r="E26">
+        <v>12122024</v>
+      </c>
+      <c r="F26" s="5">
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="G26" s="5">
+        <v>0.37708333333333333</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>37.03</v>
+      </c>
+      <c r="J26">
+        <v>0.05</v>
+      </c>
+      <c r="K26">
+        <v>23</v>
+      </c>
+      <c r="R26">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="S26">
+        <v>18933357</v>
+      </c>
+      <c r="U26" s="4">
+        <f t="shared" si="4"/>
+        <v>84.82669862583333</v>
+      </c>
+      <c r="V26" s="4">
+        <f t="shared" si="5"/>
+        <v>3.9757476135454244</v>
+      </c>
+      <c r="W26" s="4">
+        <f t="shared" si="6"/>
+        <v>4.1641123094934551</v>
+      </c>
+      <c r="X26" s="4">
+        <f t="shared" si="3"/>
+        <v>6.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="C27">
+        <v>4</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>12122024</v>
+      </c>
+      <c r="F27" s="5">
+        <v>0.36944444444444446</v>
+      </c>
+      <c r="G27" s="5">
+        <v>0.38958333333333334</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>32.93</v>
+      </c>
+      <c r="J27">
+        <v>0.05</v>
+      </c>
+      <c r="K27">
+        <v>24</v>
+      </c>
+      <c r="R27">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="S27">
+        <v>16757909</v>
+      </c>
+      <c r="U27" s="4">
+        <f t="shared" si="4"/>
+        <v>75.080087294722219</v>
+      </c>
+      <c r="V27" s="4">
+        <f t="shared" si="5"/>
+        <v>4.6858794654194593</v>
+      </c>
+      <c r="W27" s="4">
+        <f t="shared" si="6"/>
+        <v>4.7950256695738149</v>
+      </c>
+      <c r="X27" s="4">
+        <f t="shared" si="3"/>
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28">
+        <v>12122024</v>
+      </c>
+      <c r="F28" s="5">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="G28" s="5">
+        <v>0.39513888888888887</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="J28">
+        <v>0.05</v>
+      </c>
+      <c r="K28">
+        <v>23</v>
+      </c>
+      <c r="R28">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="S28">
+        <v>19532583</v>
+      </c>
+      <c r="U28" s="4">
+        <f t="shared" si="4"/>
+        <v>87.51139755749999</v>
+      </c>
+      <c r="V28" s="4">
+        <f t="shared" si="5"/>
+        <v>4.8622815128220234</v>
+      </c>
+      <c r="W28" s="4">
+        <f t="shared" si="6"/>
+        <v>5.0926487966143918</v>
+      </c>
+      <c r="X28" s="4">
+        <f t="shared" si="3"/>
+        <v>4.3999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>12122024</v>
+      </c>
+      <c r="F29" s="5">
+        <v>0.39444444444444443</v>
+      </c>
+      <c r="G29" s="5">
+        <v>0.40763888888888888</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>41.4</v>
+      </c>
+      <c r="J29">
+        <v>0.05</v>
+      </c>
+      <c r="K29">
+        <v>24</v>
+      </c>
+      <c r="R29">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="S29">
+        <v>20999312</v>
+      </c>
+      <c r="U29" s="4">
+        <f t="shared" ref="U29:U32" si="7">S29/(1200^2)*2.54^2</f>
+        <v>94.08275090222223</v>
+      </c>
+      <c r="V29" s="4">
+        <f t="shared" ref="V29:V32" si="8">I29*0.000001/18*1000/R29/(U29/10000)</f>
+        <v>4.3654578737937886</v>
+      </c>
+      <c r="W29" s="4">
+        <f t="shared" ref="W29:W32" si="9">V29/(0.88862*(1/POWER(10,(1.3272*(20-K29)-0.001053*(K29-20)^2)/(K29+105))))</f>
+        <v>4.4671406336335542</v>
+      </c>
+      <c r="X29" s="4">
+        <f t="shared" si="3"/>
+        <v>5.6000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>4</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>12122024</v>
+      </c>
+      <c r="F30" s="5">
+        <v>0.48819444444444443</v>
+      </c>
+      <c r="G30" s="5">
+        <v>0.50277777777777777</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="J30">
+        <v>0.04</v>
+      </c>
+      <c r="K30">
+        <v>24</v>
+      </c>
+      <c r="R30">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="S30">
+        <v>28234922</v>
+      </c>
+      <c r="U30" s="4">
+        <f t="shared" si="7"/>
+        <v>126.50029359388888</v>
+      </c>
+      <c r="V30" s="4">
+        <f t="shared" si="8"/>
+        <v>5.3641885666280364</v>
+      </c>
+      <c r="W30" s="4">
+        <f t="shared" si="9"/>
+        <v>5.4891343371576315</v>
+      </c>
+      <c r="X30" s="4">
+        <f t="shared" si="3"/>
+        <v>5.6000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>5</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+      <c r="E31">
+        <v>12122024</v>
+      </c>
+      <c r="F31" s="5">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="G31" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>31.9</v>
+      </c>
+      <c r="J31">
+        <v>0.03</v>
+      </c>
+      <c r="K31">
+        <v>23</v>
+      </c>
+      <c r="R31">
+        <v>0.08</v>
+      </c>
+      <c r="S31">
+        <v>15440013</v>
+      </c>
+      <c r="U31" s="4">
+        <f t="shared" si="7"/>
+        <v>69.1755471325</v>
+      </c>
+      <c r="V31" s="4">
+        <f t="shared" si="8"/>
+        <v>3.2024000815412377</v>
+      </c>
+      <c r="W31" s="4">
+        <f t="shared" si="9"/>
+        <v>3.3541247824775566</v>
+      </c>
+      <c r="X31" s="4">
+        <f t="shared" si="3"/>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>6</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="E32">
+        <v>12122024</v>
+      </c>
+      <c r="F32" s="5">
+        <v>0.50486111111111109</v>
+      </c>
+      <c r="G32" s="5">
+        <v>0.53055555555555556</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>27.76</v>
+      </c>
+      <c r="J32">
+        <v>0.06</v>
+      </c>
+      <c r="K32">
+        <v>22</v>
+      </c>
+      <c r="R32">
+        <v>3.1E-2</v>
+      </c>
+      <c r="S32">
+        <v>23530515</v>
+      </c>
+      <c r="U32" s="4">
+        <f t="shared" si="7"/>
+        <v>105.42324345416668</v>
+      </c>
+      <c r="V32" s="4">
+        <f t="shared" si="8"/>
+        <v>4.7189881768607336</v>
+      </c>
+      <c r="W32" s="4">
+        <f t="shared" si="9"/>
+        <v>5.060563198583699</v>
+      </c>
+      <c r="X32" s="4">
+        <f t="shared" si="3"/>
+        <v>3.1E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
before holiday break update just finished NAVI and some STDE no light
</commit_message>
<xml_diff>
--- a/data/Kleaf_Karli_Marion_CESE.xlsx
+++ b/data/Kleaf_Karli_Marion_CESE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marion.boisseaux\Dropbox\Mon PC (Jaboty20)\Post_doc_CalState_LA\ScoffoniLab_Kleaf\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D14C60F3-5567-4083-8E0C-E481918DE456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA48A79-0867-4064-8970-920276F0E5F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{63D1BA6E-C94C-4260-825C-85D06C6809A1}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="3" xr2:uid="{63D1BA6E-C94C-4260-825C-85D06C6809A1}"/>
   </bookViews>
   <sheets>
     <sheet name="CESE" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="DASP" sheetId="5" r:id="rId5"/>
     <sheet name="CHLA" sheetId="6" r:id="rId6"/>
     <sheet name="ZEMA" sheetId="7" r:id="rId7"/>
+    <sheet name="NAVI" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CESE!$A$1:$AE$23</definedName>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="80">
   <si>
     <t>Specie</t>
   </si>
@@ -256,6 +257,36 @@
   <si>
     <t xml:space="preserve">running cv 0.01 </t>
   </si>
+  <si>
+    <t>NAVI</t>
+  </si>
+  <si>
+    <t>leaf broke teared a little doing pressure bomb</t>
+  </si>
+  <si>
+    <t>but running cv 0.03and stable</t>
+  </si>
+  <si>
+    <t>running CV 0.07 but stable cf drawing in my notes</t>
+  </si>
+  <si>
+    <t>running cv is 0.02</t>
+  </si>
+  <si>
+    <t>leaf teared in the pressure bomb</t>
+  </si>
+  <si>
+    <t>but running cv was 0.026</t>
+  </si>
+  <si>
+    <t>but running cv was 0.01</t>
+  </si>
+  <si>
+    <t>leaf broke, noticed after the measurement</t>
+  </si>
+  <si>
+    <t>running cv 0.009</t>
+  </si>
 </sst>
 </file>
 
@@ -331,7 +362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -353,6 +384,8 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7377,10 +7410,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F80EEFC-0235-4E88-9007-0CE0804F1C9F}">
-  <dimension ref="A1:AE29"/>
+  <dimension ref="A1:AE32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
+      <selection activeCell="S33" sqref="S33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8614,7 +8647,7 @@
         <v>3.1938569589454042</v>
       </c>
       <c r="X20" s="4">
-        <f t="shared" ref="X20:X29" si="14">MAX(Q20:R20)</f>
+        <f t="shared" ref="X20:X32" si="14">MAX(Q20:R20)</f>
         <v>0.67500000000000004</v>
       </c>
     </row>
@@ -8842,15 +8875,15 @@
         <v>1849785</v>
       </c>
       <c r="U24" s="4">
-        <f t="shared" ref="U24:U29" si="15">S24/(1200^2)*2.54^2</f>
+        <f t="shared" ref="U24:U32" si="15">S24/(1200^2)*2.54^2</f>
         <v>8.2875506291666667</v>
       </c>
       <c r="V24" s="4">
-        <f t="shared" ref="V24:V29" si="16">I24*0.000001/18*1000/R24/(U24/10000)</f>
+        <f t="shared" ref="V24:V32" si="16">I24*0.000001/18*1000/R24/(U24/10000)</f>
         <v>10.18583031257724</v>
       </c>
       <c r="W24" s="4">
-        <f t="shared" ref="W24:W29" si="17">V24/(0.88862*(1/POWER(10,(1.3272*(20-K24)-0.001053*(K24-20)^2)/(K24+105))))</f>
+        <f t="shared" ref="W24:W32" si="17">V24/(0.88862*(1/POWER(10,(1.3272*(20-K24)-0.001053*(K24-20)^2)/(K24+105))))</f>
         <v>10.668419001876826</v>
       </c>
       <c r="X24" s="4">
@@ -9150,6 +9183,186 @@
       </c>
       <c r="Z29" t="s">
         <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>13</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>12192024</v>
+      </c>
+      <c r="F30" s="5">
+        <v>0.57777777777777772</v>
+      </c>
+      <c r="G30" s="5">
+        <v>0.59513888888888888</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>33.03</v>
+      </c>
+      <c r="J30">
+        <v>0.03</v>
+      </c>
+      <c r="K30">
+        <v>23</v>
+      </c>
+      <c r="R30">
+        <v>0.34599999999999997</v>
+      </c>
+      <c r="S30">
+        <v>2043504</v>
+      </c>
+      <c r="U30" s="4">
+        <f t="shared" si="15"/>
+        <v>9.1554655599999997</v>
+      </c>
+      <c r="V30" s="4">
+        <f t="shared" si="16"/>
+        <v>5.792679982614108</v>
+      </c>
+      <c r="W30" s="4">
+        <f t="shared" si="17"/>
+        <v>6.0671280889103514</v>
+      </c>
+      <c r="X30" s="4">
+        <f t="shared" si="14"/>
+        <v>0.34599999999999997</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31">
+        <v>9</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+      <c r="E31">
+        <v>12192024</v>
+      </c>
+      <c r="F31" s="5">
+        <v>0.57152777777777775</v>
+      </c>
+      <c r="G31" s="5">
+        <v>0.58888888888888891</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>35.53</v>
+      </c>
+      <c r="J31">
+        <v>0.03</v>
+      </c>
+      <c r="K31">
+        <v>23</v>
+      </c>
+      <c r="R31">
+        <v>0.435</v>
+      </c>
+      <c r="S31">
+        <v>2118510</v>
+      </c>
+      <c r="U31" s="4">
+        <f t="shared" si="15"/>
+        <v>9.4915132750000009</v>
+      </c>
+      <c r="V31" s="4">
+        <f t="shared" si="16"/>
+        <v>4.7807714904566918</v>
+      </c>
+      <c r="W31" s="4">
+        <f t="shared" si="17"/>
+        <v>5.0072769570332865</v>
+      </c>
+      <c r="X31" s="4">
+        <f t="shared" si="14"/>
+        <v>0.435</v>
+      </c>
+      <c r="Z31" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32">
+        <v>10</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>12192024</v>
+      </c>
+      <c r="F32" s="5">
+        <v>0.60347222222222219</v>
+      </c>
+      <c r="G32" s="5">
+        <v>0.62152777777777779</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>11.43</v>
+      </c>
+      <c r="J32">
+        <v>0.06</v>
+      </c>
+      <c r="K32">
+        <v>23</v>
+      </c>
+      <c r="R32">
+        <v>0.69</v>
+      </c>
+      <c r="S32">
+        <v>1508781</v>
+      </c>
+      <c r="U32" s="4">
+        <f t="shared" si="15"/>
+        <v>6.7597579858333336</v>
+      </c>
+      <c r="V32" s="4">
+        <f t="shared" si="16"/>
+        <v>1.3614242654857587</v>
+      </c>
+      <c r="W32" s="4">
+        <f t="shared" si="17"/>
+        <v>1.4259264152074329</v>
+      </c>
+      <c r="X32" s="4">
+        <f t="shared" si="14"/>
+        <v>0.69</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -14911,4 +15124,2017 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84331826-8D16-4BA7-9683-E7E875A388D4}">
+  <dimension ref="A1:AE34"/>
+  <sheetViews>
+    <sheetView topLeftCell="A37" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="U37" sqref="U37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="16" width="0" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="17.44140625" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="0" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="5.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="V1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="W1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="X1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="8">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8">
+        <v>1</v>
+      </c>
+      <c r="D2" s="8">
+        <v>2</v>
+      </c>
+      <c r="E2" s="8">
+        <v>10222024</v>
+      </c>
+      <c r="F2" s="11">
+        <v>0.50208333333333333</v>
+      </c>
+      <c r="G2" s="11">
+        <v>0.52152777777777781</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="8">
+        <v>25.26</v>
+      </c>
+      <c r="J2" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="K2" s="12" t="e">
+        <f>AVERAGE(#REF!,#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M2" s="12"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="8">
+        <v>0.155</v>
+      </c>
+      <c r="S2" s="8">
+        <f>917270+813318+608426+406146</f>
+        <v>2745160</v>
+      </c>
+      <c r="U2" s="13">
+        <f>S2/(1200^2)*2.54^2</f>
+        <v>12.299079344444445</v>
+      </c>
+      <c r="V2" s="13">
+        <f>I2*0.000001/18*1000/R2/(U2/10000)</f>
+        <v>7.3613342814556653</v>
+      </c>
+      <c r="W2" s="13" t="e">
+        <f>V2/(0.88862*(1/POWER(10,(1.3272*(20-K2)-0.001053*(K2-20)^2)/(K2+105))))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="X2" s="13">
+        <f>MAX(Q2:R2)</f>
+        <v>0.155</v>
+      </c>
+      <c r="Z2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB2" s="14"/>
+      <c r="AC2" s="14"/>
+      <c r="AD2" s="13"/>
+      <c r="AE2" s="13"/>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>12172024</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0.41249999999999998</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3">
+        <v>143.13</v>
+      </c>
+      <c r="J3">
+        <v>0.01</v>
+      </c>
+      <c r="K3">
+        <v>24</v>
+      </c>
+      <c r="R3">
+        <v>0.156</v>
+      </c>
+      <c r="S3">
+        <v>2207061</v>
+      </c>
+      <c r="U3" s="16">
+        <f t="shared" ref="U3:U31" si="0">S3/(1200^2)*2.54^2</f>
+        <v>9.8882463524999995</v>
+      </c>
+      <c r="V3" s="16">
+        <f t="shared" ref="V3:V31" si="1">I3*0.000001/18*1000/R3/(U3/10000)</f>
+        <v>51.548293200983167</v>
+      </c>
+      <c r="W3" s="16">
+        <f t="shared" ref="W3:W31" si="2">V3/(0.88862*(1/POWER(10,(1.3272*(20-K3)-0.001053*(K3-20)^2)/(K3+105))))</f>
+        <v>52.748985744409367</v>
+      </c>
+      <c r="X3" s="16">
+        <f t="shared" ref="X3:X34" si="3">MAX(Q3:R3)</f>
+        <v>0.156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>12172024</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0.41041666666666665</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="H4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4">
+        <v>69.37</v>
+      </c>
+      <c r="J4">
+        <v>0.02</v>
+      </c>
+      <c r="K4">
+        <v>25</v>
+      </c>
+      <c r="R4">
+        <v>2.2149999999999999</v>
+      </c>
+      <c r="S4">
+        <v>2386921</v>
+      </c>
+      <c r="U4" s="16">
+        <f t="shared" si="0"/>
+        <v>10.694069113611111</v>
+      </c>
+      <c r="V4" s="16">
+        <f t="shared" si="1"/>
+        <v>1.626980966514223</v>
+      </c>
+      <c r="W4" s="16">
+        <f t="shared" si="2"/>
+        <v>1.6271130746564908</v>
+      </c>
+      <c r="X4" s="16">
+        <f t="shared" si="3"/>
+        <v>2.2149999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>12172024</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0.43125000000000002</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0.46388888888888891</v>
+      </c>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5">
+        <v>40.97</v>
+      </c>
+      <c r="J5">
+        <v>0.05</v>
+      </c>
+      <c r="K5">
+        <v>25</v>
+      </c>
+      <c r="R5">
+        <v>1.9770000000000001</v>
+      </c>
+      <c r="S5">
+        <v>2439568</v>
+      </c>
+      <c r="U5" s="16">
+        <f t="shared" si="0"/>
+        <v>10.929942297777778</v>
+      </c>
+      <c r="V5" s="16">
+        <f t="shared" si="1"/>
+        <v>1.0533408337409196</v>
+      </c>
+      <c r="W5" s="16">
+        <f t="shared" si="2"/>
+        <v>1.0534263632606768</v>
+      </c>
+      <c r="X5" s="16">
+        <f t="shared" si="3"/>
+        <v>1.9770000000000001</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>12172024</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0.45208333333333334</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0.47152777777777777</v>
+      </c>
+      <c r="H6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6">
+        <v>187.4</v>
+      </c>
+      <c r="J6">
+        <v>0.02</v>
+      </c>
+      <c r="K6">
+        <v>24</v>
+      </c>
+      <c r="R6">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="S6">
+        <v>3283581</v>
+      </c>
+      <c r="U6" s="16">
+        <f t="shared" si="0"/>
+        <v>14.711354985833335</v>
+      </c>
+      <c r="V6" s="16">
+        <f t="shared" si="1"/>
+        <v>85.264119959470463</v>
+      </c>
+      <c r="W6" s="16">
+        <f t="shared" si="2"/>
+        <v>87.25014096423925</v>
+      </c>
+      <c r="X6" s="16">
+        <f t="shared" si="3"/>
+        <v>8.3000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>12172024</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0.47708333333333336</v>
+      </c>
+      <c r="G7" s="5">
+        <v>0.51249999999999996</v>
+      </c>
+      <c r="H7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7">
+        <v>16.7</v>
+      </c>
+      <c r="J7">
+        <v>0.09</v>
+      </c>
+      <c r="K7">
+        <v>25</v>
+      </c>
+      <c r="R7">
+        <v>1.5549999999999999</v>
+      </c>
+      <c r="S7">
+        <v>1968755</v>
+      </c>
+      <c r="U7" s="16">
+        <f t="shared" si="0"/>
+        <v>8.8205692763888894</v>
+      </c>
+      <c r="V7" s="16">
+        <f t="shared" si="1"/>
+        <v>0.67642080577725283</v>
+      </c>
+      <c r="W7" s="16">
+        <f t="shared" si="2"/>
+        <v>0.67647573001907346</v>
+      </c>
+      <c r="X7" s="16">
+        <f t="shared" si="3"/>
+        <v>1.5549999999999999</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>12172024</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0.50208333333333333</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0.5180555555555556</v>
+      </c>
+      <c r="H8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8">
+        <v>74.83</v>
+      </c>
+      <c r="J8">
+        <v>0.03</v>
+      </c>
+      <c r="K8">
+        <v>24</v>
+      </c>
+      <c r="R8">
+        <v>0.44600000000000001</v>
+      </c>
+      <c r="S8">
+        <v>1823104</v>
+      </c>
+      <c r="U8" s="16">
+        <f t="shared" si="0"/>
+        <v>8.1680123377777782</v>
+      </c>
+      <c r="V8" s="16">
+        <f t="shared" si="1"/>
+        <v>11.411743363416814</v>
+      </c>
+      <c r="W8" s="16">
+        <f t="shared" si="2"/>
+        <v>11.677552264412331</v>
+      </c>
+      <c r="X8" s="16">
+        <f t="shared" si="3"/>
+        <v>0.44600000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>12172024</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0.53055555555555556</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0.54374999999999996</v>
+      </c>
+      <c r="H9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9">
+        <v>89.73</v>
+      </c>
+      <c r="J9">
+        <v>0.02</v>
+      </c>
+      <c r="K9">
+        <v>25</v>
+      </c>
+      <c r="R9">
+        <v>2.11</v>
+      </c>
+      <c r="S9">
+        <v>4184197</v>
+      </c>
+      <c r="U9" s="16">
+        <f t="shared" si="0"/>
+        <v>18.746364836944444</v>
+      </c>
+      <c r="V9" s="16">
+        <f t="shared" si="1"/>
+        <v>1.2602759320303754</v>
+      </c>
+      <c r="W9" s="16">
+        <f t="shared" si="2"/>
+        <v>1.2603782643351484</v>
+      </c>
+      <c r="X9" s="16">
+        <f t="shared" si="3"/>
+        <v>2.11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>12172024</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0.54861111111111116</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0.57013888888888886</v>
+      </c>
+      <c r="H10" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10">
+        <v>99.78</v>
+      </c>
+      <c r="J10">
+        <v>0.05</v>
+      </c>
+      <c r="K10">
+        <v>24</v>
+      </c>
+      <c r="R10">
+        <v>1.85</v>
+      </c>
+      <c r="S10">
+        <v>2933375</v>
+      </c>
+      <c r="U10" s="16">
+        <f t="shared" si="0"/>
+        <v>13.14233482638889</v>
+      </c>
+      <c r="V10" s="16">
+        <f t="shared" si="1"/>
+        <v>2.2799574322059133</v>
+      </c>
+      <c r="W10" s="16">
+        <f t="shared" si="2"/>
+        <v>2.3330635142541656</v>
+      </c>
+      <c r="X10" s="16">
+        <f t="shared" si="3"/>
+        <v>1.85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>12172024</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="G11" s="5">
+        <v>0.57013888888888886</v>
+      </c>
+      <c r="H11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11">
+        <v>43.93</v>
+      </c>
+      <c r="J11">
+        <v>0.04</v>
+      </c>
+      <c r="K11">
+        <f>AVERAGE(K3:K10,K12:K15)</f>
+        <v>24.5</v>
+      </c>
+      <c r="R11">
+        <v>0.11</v>
+      </c>
+      <c r="S11">
+        <v>1471589</v>
+      </c>
+      <c r="U11" s="16">
+        <f t="shared" si="0"/>
+        <v>6.5931274947222223</v>
+      </c>
+      <c r="V11" s="16">
+        <f t="shared" si="1"/>
+        <v>33.651508642338861</v>
+      </c>
+      <c r="W11" s="16">
+        <f t="shared" si="2"/>
+        <v>34.04120133348399</v>
+      </c>
+      <c r="X11" s="16">
+        <f t="shared" si="3"/>
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>12172024</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0.57777777777777772</v>
+      </c>
+      <c r="G12" s="5">
+        <v>0.6020833333333333</v>
+      </c>
+      <c r="H12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" s="5">
+        <v>0.49513888888888891</v>
+      </c>
+      <c r="J12" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="K12" s="15">
+        <v>25</v>
+      </c>
+      <c r="R12">
+        <v>2.8</v>
+      </c>
+      <c r="S12">
+        <v>2824028</v>
+      </c>
+      <c r="U12" s="16">
+        <f t="shared" si="0"/>
+        <v>12.652429892222223</v>
+      </c>
+      <c r="V12" s="16">
+        <f t="shared" si="1"/>
+        <v>7.7646621139471021E-3</v>
+      </c>
+      <c r="W12" s="16">
+        <f t="shared" si="2"/>
+        <v>7.765292591566891E-3</v>
+      </c>
+      <c r="X12" s="16">
+        <f t="shared" si="3"/>
+        <v>2.8</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>12172024</v>
+      </c>
+      <c r="F13" s="5">
+        <v>0.57986111111111116</v>
+      </c>
+      <c r="G13" s="5">
+        <v>0.59444444444444444</v>
+      </c>
+      <c r="H13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13">
+        <v>77.63</v>
+      </c>
+      <c r="J13" s="15">
+        <v>0.04</v>
+      </c>
+      <c r="K13" s="15">
+        <v>24</v>
+      </c>
+      <c r="R13">
+        <v>1.33</v>
+      </c>
+      <c r="S13">
+        <v>2058880</v>
+      </c>
+      <c r="U13" s="16">
+        <f t="shared" si="0"/>
+        <v>9.2243543111111119</v>
+      </c>
+      <c r="V13" s="16">
+        <f t="shared" si="1"/>
+        <v>3.5153572262218704</v>
+      </c>
+      <c r="W13" s="16">
+        <f t="shared" si="2"/>
+        <v>3.5972389520153345</v>
+      </c>
+      <c r="X13" s="16">
+        <f t="shared" si="3"/>
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14" s="15">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>12172024</v>
+      </c>
+      <c r="F14" s="5">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="G14" s="5">
+        <v>0.63194444444444442</v>
+      </c>
+      <c r="H14" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" s="15">
+        <v>19.07</v>
+      </c>
+      <c r="J14" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="K14" s="15">
+        <v>25</v>
+      </c>
+      <c r="R14">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="S14">
+        <v>1954502</v>
+      </c>
+      <c r="U14" s="16">
+        <f t="shared" si="0"/>
+        <v>8.756711877222223</v>
+      </c>
+      <c r="V14" s="16">
+        <f t="shared" si="1"/>
+        <v>0.52149379187689426</v>
+      </c>
+      <c r="W14" s="16">
+        <f t="shared" si="2"/>
+        <v>0.52153613630345297</v>
+      </c>
+      <c r="X14" s="16">
+        <f t="shared" si="3"/>
+        <v>2.3199999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>12172024</v>
+      </c>
+      <c r="F15" s="5">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="G15" s="5">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="H15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15" s="15">
+        <v>86.37</v>
+      </c>
+      <c r="J15" s="15">
+        <v>0.02</v>
+      </c>
+      <c r="K15" s="15">
+        <v>24</v>
+      </c>
+      <c r="R15">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="S15">
+        <v>2228321</v>
+      </c>
+      <c r="U15" s="16">
+        <f t="shared" si="0"/>
+        <v>9.9834970580555549</v>
+      </c>
+      <c r="V15" s="16">
+        <f t="shared" si="1"/>
+        <v>49.549124584531697</v>
+      </c>
+      <c r="W15" s="16">
+        <f t="shared" si="2"/>
+        <v>50.70325134077526</v>
+      </c>
+      <c r="X15" s="16">
+        <f t="shared" si="3"/>
+        <v>9.7000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>7</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>12182024</v>
+      </c>
+      <c r="F16" s="5">
+        <v>0.37361111111111112</v>
+      </c>
+      <c r="G16" s="5">
+        <v>0.39027777777777778</v>
+      </c>
+      <c r="H16" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16" s="15">
+        <v>105.78</v>
+      </c>
+      <c r="J16" s="15">
+        <v>0.02</v>
+      </c>
+      <c r="K16" s="15">
+        <v>24</v>
+      </c>
+      <c r="R16">
+        <v>1.94</v>
+      </c>
+      <c r="S16">
+        <v>3496221</v>
+      </c>
+      <c r="U16" s="16">
+        <f t="shared" si="0"/>
+        <v>15.664041252499999</v>
+      </c>
+      <c r="V16" s="16">
+        <f t="shared" si="1"/>
+        <v>1.933862132487465</v>
+      </c>
+      <c r="W16" s="16">
+        <f t="shared" si="2"/>
+        <v>1.9789067634210009</v>
+      </c>
+      <c r="X16" s="16">
+        <f t="shared" si="3"/>
+        <v>1.94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>6</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>12182024</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0.38263888888888886</v>
+      </c>
+      <c r="G17" s="5">
+        <v>0.39861111111111114</v>
+      </c>
+      <c r="H17" t="s">
+        <v>28</v>
+      </c>
+      <c r="I17" s="15">
+        <v>26.8</v>
+      </c>
+      <c r="J17" s="15">
+        <v>0.03</v>
+      </c>
+      <c r="K17" s="15">
+        <v>25</v>
+      </c>
+      <c r="R17">
+        <v>2</v>
+      </c>
+      <c r="S17">
+        <v>2294812</v>
+      </c>
+      <c r="U17" s="16">
+        <f t="shared" si="0"/>
+        <v>10.281395207777779</v>
+      </c>
+      <c r="V17" s="16">
+        <f t="shared" si="1"/>
+        <v>0.72406947636958763</v>
+      </c>
+      <c r="W17" s="16">
+        <f t="shared" si="2"/>
+        <v>0.72412826960402898</v>
+      </c>
+      <c r="X17" s="16">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>7</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>12182024</v>
+      </c>
+      <c r="F18" s="5">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="G18" s="5">
+        <v>0.45</v>
+      </c>
+      <c r="H18" t="s">
+        <v>28</v>
+      </c>
+      <c r="I18" s="15">
+        <v>124.17</v>
+      </c>
+      <c r="J18" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="K18" s="15">
+        <v>24</v>
+      </c>
+      <c r="R18">
+        <v>1.98</v>
+      </c>
+      <c r="S18">
+        <v>4142713</v>
+      </c>
+      <c r="U18" s="16">
+        <f t="shared" si="0"/>
+        <v>18.560504993611112</v>
+      </c>
+      <c r="V18" s="16">
+        <f t="shared" si="1"/>
+        <v>1.8771077269750995</v>
+      </c>
+      <c r="W18" s="16">
+        <f t="shared" si="2"/>
+        <v>1.9208304015978883</v>
+      </c>
+      <c r="X18" s="16">
+        <f t="shared" si="3"/>
+        <v>1.98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>7</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>12182024</v>
+      </c>
+      <c r="F19" s="5">
+        <v>0.43819444444444444</v>
+      </c>
+      <c r="G19" s="5">
+        <v>0.46180555555555558</v>
+      </c>
+      <c r="H19" t="s">
+        <v>28</v>
+      </c>
+      <c r="I19" s="15">
+        <v>30.9</v>
+      </c>
+      <c r="J19" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="K19" s="15">
+        <v>25</v>
+      </c>
+      <c r="R19">
+        <v>2.11</v>
+      </c>
+      <c r="S19">
+        <v>1448956</v>
+      </c>
+      <c r="U19" s="16">
+        <f t="shared" si="0"/>
+        <v>6.4917253677777786</v>
+      </c>
+      <c r="V19" s="16">
+        <f t="shared" si="1"/>
+        <v>1.2532663534791386</v>
+      </c>
+      <c r="W19" s="16">
+        <f t="shared" si="2"/>
+        <v>1.2533681166178183</v>
+      </c>
+      <c r="X19" s="16">
+        <f t="shared" si="3"/>
+        <v>2.11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>8</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <v>12182024</v>
+      </c>
+      <c r="F20" s="5">
+        <v>0.46527777777777779</v>
+      </c>
+      <c r="G20" s="5">
+        <v>0.48125000000000001</v>
+      </c>
+      <c r="H20" t="s">
+        <v>28</v>
+      </c>
+      <c r="I20" s="15">
+        <v>64.900000000000006</v>
+      </c>
+      <c r="J20" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="K20" s="15">
+        <v>26</v>
+      </c>
+      <c r="R20">
+        <v>2.11</v>
+      </c>
+      <c r="S20">
+        <v>2674281</v>
+      </c>
+      <c r="U20" s="16">
+        <f t="shared" si="0"/>
+        <v>11.981521735833333</v>
+      </c>
+      <c r="V20" s="16">
+        <f t="shared" si="1"/>
+        <v>1.4261912132984851</v>
+      </c>
+      <c r="W20" s="16">
+        <f t="shared" si="2"/>
+        <v>1.3943908123683739</v>
+      </c>
+      <c r="X20" s="16">
+        <f t="shared" si="3"/>
+        <v>2.11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>9</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>12182024</v>
+      </c>
+      <c r="F21" s="5">
+        <v>0.46944444444444444</v>
+      </c>
+      <c r="G21" s="5">
+        <v>0.48888888888888887</v>
+      </c>
+      <c r="H21" t="s">
+        <v>28</v>
+      </c>
+      <c r="I21" s="15">
+        <v>102.18</v>
+      </c>
+      <c r="J21" s="15">
+        <v>0.02</v>
+      </c>
+      <c r="R21">
+        <v>1.06</v>
+      </c>
+      <c r="S21">
+        <f>3440799</f>
+        <v>3440799</v>
+      </c>
+      <c r="U21" s="16">
+        <f t="shared" si="0"/>
+        <v>15.415735297499999</v>
+      </c>
+      <c r="V21" s="16">
+        <f t="shared" si="1"/>
+        <v>3.4739477609077603</v>
+      </c>
+      <c r="W21" s="16">
+        <f t="shared" si="2"/>
+        <v>6.932594070059837</v>
+      </c>
+      <c r="X21" s="16">
+        <f t="shared" si="3"/>
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>8</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>12182024</v>
+      </c>
+      <c r="F22" s="5">
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="G22" s="5">
+        <v>0.51458333333333328</v>
+      </c>
+      <c r="H22" t="s">
+        <v>28</v>
+      </c>
+      <c r="I22" s="15">
+        <v>119.5</v>
+      </c>
+      <c r="J22" s="15">
+        <v>0.02</v>
+      </c>
+      <c r="K22" s="15">
+        <v>25</v>
+      </c>
+      <c r="R22">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="S22">
+        <v>2544666</v>
+      </c>
+      <c r="U22" s="16">
+        <f t="shared" si="0"/>
+        <v>11.400810531666666</v>
+      </c>
+      <c r="V22" s="16">
+        <f t="shared" si="1"/>
+        <v>21.09845188882462</v>
+      </c>
+      <c r="W22" s="16">
+        <f t="shared" si="2"/>
+        <v>21.100165047946408</v>
+      </c>
+      <c r="X22" s="16">
+        <f t="shared" si="3"/>
+        <v>0.27600000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="C23">
+        <v>9</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23">
+        <v>12182024</v>
+      </c>
+      <c r="F23" s="5">
+        <v>0.49652777777777779</v>
+      </c>
+      <c r="G23" s="5">
+        <v>0.51180555555555551</v>
+      </c>
+      <c r="H23" t="s">
+        <v>28</v>
+      </c>
+      <c r="I23" s="15">
+        <v>74.900000000000006</v>
+      </c>
+      <c r="J23" s="15">
+        <v>0.04</v>
+      </c>
+      <c r="K23" s="15">
+        <v>24</v>
+      </c>
+      <c r="R23">
+        <v>1.7749999999999999</v>
+      </c>
+      <c r="S23">
+        <v>3639298</v>
+      </c>
+      <c r="U23" s="16">
+        <f t="shared" si="0"/>
+        <v>16.305065956111111</v>
+      </c>
+      <c r="V23" s="16">
+        <f t="shared" si="1"/>
+        <v>1.4377666157450395</v>
+      </c>
+      <c r="W23" s="16">
+        <f t="shared" si="2"/>
+        <v>1.4712559040902695</v>
+      </c>
+      <c r="X23" s="16">
+        <f t="shared" si="3"/>
+        <v>1.7749999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24">
+        <v>10</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24">
+        <v>12182024</v>
+      </c>
+      <c r="F24" s="5">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G24" s="5">
+        <v>0.56388888888888888</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24" s="15">
+        <v>17.93</v>
+      </c>
+      <c r="J24" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="K24" s="15">
+        <v>23</v>
+      </c>
+      <c r="R24">
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="S24">
+        <v>2354118</v>
+      </c>
+      <c r="U24" s="16">
+        <f t="shared" si="0"/>
+        <v>10.547102561666666</v>
+      </c>
+      <c r="V24" s="16">
+        <f t="shared" si="1"/>
+        <v>1.2345627815630753</v>
+      </c>
+      <c r="W24" s="16">
+        <f t="shared" si="2"/>
+        <v>1.2930544328403317</v>
+      </c>
+      <c r="X24" s="16">
+        <f t="shared" si="3"/>
+        <v>0.76500000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>10</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>12182024</v>
+      </c>
+      <c r="F25" s="5">
+        <v>0.55694444444444446</v>
+      </c>
+      <c r="G25" s="5">
+        <v>0.57777777777777772</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25" s="15">
+        <v>12.23</v>
+      </c>
+      <c r="J25" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="K25" s="15">
+        <v>24</v>
+      </c>
+      <c r="R25">
+        <v>0.23699999999999999</v>
+      </c>
+      <c r="S25">
+        <v>2170297</v>
+      </c>
+      <c r="U25" s="16">
+        <f t="shared" si="0"/>
+        <v>9.7235334202777768</v>
+      </c>
+      <c r="V25" s="16">
+        <f t="shared" si="1"/>
+        <v>2.9483666811793827</v>
+      </c>
+      <c r="W25" s="16">
+        <f t="shared" si="2"/>
+        <v>3.017041736541076</v>
+      </c>
+      <c r="X25" s="16">
+        <f t="shared" si="3"/>
+        <v>0.23699999999999999</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>11</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+      <c r="E26">
+        <v>12182024</v>
+      </c>
+      <c r="F26" s="5">
+        <v>0.56805555555555554</v>
+      </c>
+      <c r="G26" s="5">
+        <v>0.58263888888888893</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26" s="15">
+        <v>58.03</v>
+      </c>
+      <c r="J26" s="15">
+        <v>0.04</v>
+      </c>
+      <c r="K26" s="15">
+        <v>23</v>
+      </c>
+      <c r="R26">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="S26">
+        <v>2648266</v>
+      </c>
+      <c r="U26" s="16">
+        <f t="shared" si="0"/>
+        <v>11.864967309444443</v>
+      </c>
+      <c r="V26" s="16">
+        <f t="shared" si="1"/>
+        <v>37.22122475337563</v>
+      </c>
+      <c r="W26" s="16">
+        <f t="shared" si="2"/>
+        <v>38.984708094117828</v>
+      </c>
+      <c r="X26" s="16">
+        <f t="shared" si="3"/>
+        <v>7.2999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>9</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="E27">
+        <v>12182024</v>
+      </c>
+      <c r="F27" s="5">
+        <v>0.58680555555555558</v>
+      </c>
+      <c r="G27" s="5">
+        <v>0.60486111111111107</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27" s="15">
+        <v>8.83</v>
+      </c>
+      <c r="J27" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="K27" s="15">
+        <v>24</v>
+      </c>
+      <c r="R27">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="S27">
+        <v>1084842</v>
+      </c>
+      <c r="U27" s="16">
+        <f t="shared" si="0"/>
+        <v>4.8603935050000002</v>
+      </c>
+      <c r="V27" s="16">
+        <f t="shared" si="1"/>
+        <v>1.8023068761632366</v>
+      </c>
+      <c r="W27" s="16">
+        <f t="shared" si="2"/>
+        <v>1.8442872462743791</v>
+      </c>
+      <c r="X27" s="16">
+        <f t="shared" si="3"/>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>70</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <v>11</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28">
+        <v>12192024</v>
+      </c>
+      <c r="F28" s="5">
+        <v>0.40555555555555556</v>
+      </c>
+      <c r="G28" s="5">
+        <v>0.41805555555555557</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28" s="15">
+        <v>36.4</v>
+      </c>
+      <c r="J28" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="K28" s="15">
+        <v>23</v>
+      </c>
+      <c r="R28">
+        <v>0.67300000000000004</v>
+      </c>
+      <c r="S28">
+        <v>1964981</v>
+      </c>
+      <c r="U28" s="16">
+        <f t="shared" si="0"/>
+        <v>8.8036607080555562</v>
+      </c>
+      <c r="V28" s="16">
+        <f t="shared" si="1"/>
+        <v>3.4131118274703223</v>
+      </c>
+      <c r="W28" s="16">
+        <f t="shared" si="2"/>
+        <v>3.5748197209562349</v>
+      </c>
+      <c r="X28" s="16">
+        <f t="shared" si="3"/>
+        <v>0.67300000000000004</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <v>12</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="F29" s="5">
+        <v>0.42222222222222222</v>
+      </c>
+      <c r="G29" s="5">
+        <v>0.43611111111111112</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29" s="15">
+        <v>20.63</v>
+      </c>
+      <c r="J29" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="K29" s="15">
+        <v>23</v>
+      </c>
+      <c r="R29">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="S29">
+        <v>2853960</v>
+      </c>
+      <c r="U29" s="16">
+        <f t="shared" si="0"/>
+        <v>12.786533566666668</v>
+      </c>
+      <c r="V29" s="16">
+        <f t="shared" si="1"/>
+        <v>4.6203212166372989</v>
+      </c>
+      <c r="W29" s="16">
+        <f t="shared" si="2"/>
+        <v>4.8392248005038851</v>
+      </c>
+      <c r="X29" s="16">
+        <f t="shared" si="3"/>
+        <v>0.19400000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>10</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="F30" s="5">
+        <v>0.43611111111111112</v>
+      </c>
+      <c r="G30" s="5">
+        <v>0.45416666666666666</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30" s="15">
+        <v>23.16</v>
+      </c>
+      <c r="J30" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="K30" s="15">
+        <v>23</v>
+      </c>
+      <c r="R30">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="S30">
+        <v>2559226</v>
+      </c>
+      <c r="U30" s="16">
+        <f t="shared" si="0"/>
+        <v>11.466043376111111</v>
+      </c>
+      <c r="V30" s="16">
+        <f t="shared" si="1"/>
+        <v>8.4372482698040336</v>
+      </c>
+      <c r="W30" s="16">
+        <f t="shared" si="2"/>
+        <v>8.8369918801793474</v>
+      </c>
+      <c r="X30" s="16">
+        <f t="shared" si="3"/>
+        <v>0.13300000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>11</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+      <c r="F31" s="5">
+        <v>0.44166666666666665</v>
+      </c>
+      <c r="G31" s="5">
+        <v>0.47083333333333333</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31" s="15">
+        <v>7.67</v>
+      </c>
+      <c r="J31" s="15">
+        <v>0.17</v>
+      </c>
+      <c r="K31" s="15">
+        <v>22</v>
+      </c>
+      <c r="R31">
+        <v>2.17</v>
+      </c>
+      <c r="S31">
+        <v>1549126</v>
+      </c>
+      <c r="U31" s="16">
+        <f t="shared" si="0"/>
+        <v>6.9405147927777779</v>
+      </c>
+      <c r="V31" s="16">
+        <f t="shared" si="1"/>
+        <v>0.28292507572585829</v>
+      </c>
+      <c r="W31" s="16">
+        <f t="shared" si="2"/>
+        <v>0.3034040714904378</v>
+      </c>
+      <c r="X31" s="16">
+        <f t="shared" si="3"/>
+        <v>2.17</v>
+      </c>
+      <c r="Z31" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32">
+        <v>13</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="F32" s="5">
+        <v>0.46180555555555558</v>
+      </c>
+      <c r="G32" s="5">
+        <v>0.47569444444444442</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32" s="15">
+        <v>26.43</v>
+      </c>
+      <c r="J32" s="15">
+        <v>0.04</v>
+      </c>
+      <c r="K32" s="15">
+        <v>23</v>
+      </c>
+      <c r="R32">
+        <v>0.156</v>
+      </c>
+      <c r="S32">
+        <v>1676287</v>
+      </c>
+      <c r="U32" s="16">
+        <f t="shared" ref="U32:U34" si="4">S32/(1200^2)*2.54^2</f>
+        <v>7.5102313952777768</v>
+      </c>
+      <c r="V32" s="16">
+        <f t="shared" ref="V32:V34" si="5">I32*0.000001/18*1000/R32/(U32/10000)</f>
+        <v>12.532760532932997</v>
+      </c>
+      <c r="W32" s="16">
+        <f t="shared" ref="W32:W34" si="6">V32/(0.88862*(1/POWER(10,(1.3272*(20-K32)-0.001053*(K32-20)^2)/(K32+105))))</f>
+        <v>13.126543100803344</v>
+      </c>
+      <c r="X32" s="16">
+        <f t="shared" si="3"/>
+        <v>0.156</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33">
+        <v>13</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="F33" s="5">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="G33" s="5">
+        <v>0.49513888888888891</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33" s="15">
+        <v>18.3</v>
+      </c>
+      <c r="J33" s="15">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K33" s="15">
+        <v>23</v>
+      </c>
+      <c r="R33">
+        <v>7.8E-2</v>
+      </c>
+      <c r="S33">
+        <v>1908448</v>
+      </c>
+      <c r="U33" s="16">
+        <f t="shared" si="4"/>
+        <v>8.5503771644444448</v>
+      </c>
+      <c r="V33" s="16">
+        <f t="shared" si="5"/>
+        <v>15.243991912297034</v>
+      </c>
+      <c r="W33" s="16">
+        <f t="shared" si="6"/>
+        <v>15.966228377159911</v>
+      </c>
+      <c r="X33" s="16">
+        <f t="shared" si="3"/>
+        <v>7.8E-2</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>70</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34">
+        <v>14</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="F34" s="5">
+        <v>0.4777777777777778</v>
+      </c>
+      <c r="G34" s="5">
+        <v>0.50138888888888888</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34" s="15">
+        <v>20.73</v>
+      </c>
+      <c r="J34" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="K34" s="15">
+        <v>22</v>
+      </c>
+      <c r="R34">
+        <v>0.86899999999999999</v>
+      </c>
+      <c r="S34">
+        <v>2717664</v>
+      </c>
+      <c r="U34" s="16">
+        <f t="shared" si="4"/>
+        <v>12.175889626666667</v>
+      </c>
+      <c r="V34" s="16">
+        <f t="shared" si="5"/>
+        <v>1.0884445720725633</v>
+      </c>
+      <c r="W34" s="16">
+        <f t="shared" si="6"/>
+        <v>1.1672295709782519</v>
+      </c>
+      <c r="X34" s="16">
+        <f t="shared" si="3"/>
+        <v>0.86899999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>